<commit_message>
GS 7 and TS 7 Padam Templates 12/07/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1201E933-D54A-4B24-A237-4F442C19E1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2083A1-C6EE-4C5D-8D7C-7A726558821E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6841" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6980" uniqueCount="1184">
   <si>
     <t>Passage</t>
   </si>
@@ -3502,19 +3502,103 @@
   </si>
   <si>
     <t>svAhetiq svAhA$ ||</t>
+  </si>
+  <si>
+    <t>GS-7.3-01</t>
+  </si>
+  <si>
+    <t>GS-7.3-02</t>
+  </si>
+  <si>
+    <t>GS-7.3-03</t>
+  </si>
+  <si>
+    <t>GS-7.3-04</t>
+  </si>
+  <si>
+    <t>GS-7.3-05</t>
+  </si>
+  <si>
+    <t>GS-7.3-06</t>
+  </si>
+  <si>
+    <t>GS-7.3-07</t>
+  </si>
+  <si>
+    <t>ngg</t>
+  </si>
+  <si>
+    <t>P[S]</t>
+  </si>
+  <si>
+    <t>GS-7.3-08</t>
+  </si>
+  <si>
+    <t>S[s]</t>
+  </si>
+  <si>
+    <t>GS-7.3-09</t>
+  </si>
+  <si>
+    <t>GS-7.3-10</t>
+  </si>
+  <si>
+    <t>Kampam</t>
+  </si>
+  <si>
+    <t>GS-7.3-11</t>
+  </si>
+  <si>
+    <t>vis%N</t>
+  </si>
+  <si>
+    <t>P[Sh]+N</t>
+  </si>
+  <si>
+    <t>GS-7.3-12</t>
+  </si>
+  <si>
+    <t>GS-7.3-13</t>
+  </si>
+  <si>
+    <t>Vis%N</t>
+  </si>
+  <si>
+    <t>GS-7.3-14</t>
+  </si>
+  <si>
+    <t>GS-7.3-15</t>
+  </si>
+  <si>
+    <t>GS-7.3-16</t>
+  </si>
+  <si>
+    <t>GS-7.3-17</t>
+  </si>
+  <si>
+    <t>GS-7.3-18</t>
+  </si>
+  <si>
+    <t>GS-7.3-19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3680,185 +3764,188 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4142,20 +4229,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1575" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1775" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="V1588" sqref="V1588"/>
+      <selection pane="bottomLeft" activeCell="N1781" sqref="N1781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="5" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="30" hidden="1" customWidth="1"/>
-    <col min="5" max="7" width="11.28515625" style="5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="30" customWidth="1"/>
+    <col min="5" max="7" width="11.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="9" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" style="4" customWidth="1"/>
@@ -4163,12 +4250,11 @@
     <col min="13" max="13" width="16.28515625" style="6" customWidth="1"/>
     <col min="14" max="14" width="45.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="3" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="6.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="23.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="17" width="5.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" style="1" customWidth="1"/>
     <col min="22" max="22" width="76.7109375" style="55" bestFit="1" customWidth="1"/>
     <col min="23" max="262" width="9.140625" style="2"/>
     <col min="263" max="263" width="9.28515625" style="2" customWidth="1"/>
@@ -6501,7 +6587,9 @@
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
+      <c r="H46" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I46" s="59" t="s">
         <v>20</v>
       </c>
@@ -6542,7 +6630,9 @@
       <c r="E47" s="25"/>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
+      <c r="H47" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I47" s="59" t="s">
         <v>20</v>
       </c>
@@ -6583,7 +6673,9 @@
       <c r="E48" s="25"/>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I48" s="59" t="s">
         <v>20</v>
       </c>
@@ -6622,7 +6714,9 @@
       <c r="E49" s="25"/>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I49" s="59" t="s">
         <v>20</v>
       </c>
@@ -6660,7 +6754,9 @@
       <c r="E50" s="24"/>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
+      <c r="H50" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I50" s="59" t="s">
         <v>20</v>
       </c>
@@ -6703,7 +6799,9 @@
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
+      <c r="H51" s="61" t="s">
+        <v>1159</v>
+      </c>
       <c r="I51" s="59" t="s">
         <v>20</v>
       </c>
@@ -6823,7 +6921,6 @@
       <c r="E54" s="25"/>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="41"/>
       <c r="I54" s="59" t="s">
         <v>21</v>
       </c>
@@ -6864,7 +6961,7 @@
       <c r="E55" s="25"/>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="41"/>
+      <c r="H55" s="61"/>
       <c r="I55" s="59" t="s">
         <v>21</v>
       </c>
@@ -6905,7 +7002,7 @@
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
-      <c r="H56" s="41"/>
+      <c r="H56" s="61"/>
       <c r="I56" s="59" t="s">
         <v>21</v>
       </c>
@@ -6948,7 +7045,7 @@
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="41"/>
+      <c r="H57" s="61"/>
       <c r="I57" s="59" t="s">
         <v>21</v>
       </c>
@@ -6991,7 +7088,7 @@
       <c r="E58" s="25"/>
       <c r="F58" s="25"/>
       <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
+      <c r="H58" s="61"/>
       <c r="I58" s="59" t="s">
         <v>21</v>
       </c>
@@ -7032,7 +7129,7 @@
       <c r="E59" s="25"/>
       <c r="F59" s="25"/>
       <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="H59" s="61"/>
       <c r="I59" s="59" t="s">
         <v>21</v>
       </c>
@@ -7073,7 +7170,7 @@
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
       <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
+      <c r="H60" s="61"/>
       <c r="I60" s="59" t="s">
         <v>21</v>
       </c>
@@ -7113,7 +7210,7 @@
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
+      <c r="H61" s="61"/>
       <c r="I61" s="59" t="s">
         <v>21</v>
       </c>
@@ -7151,7 +7248,7 @@
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
+      <c r="H62" s="61"/>
       <c r="I62" s="59" t="s">
         <v>21</v>
       </c>
@@ -8262,7 +8359,9 @@
       <c r="E90" s="24"/>
       <c r="F90" s="24"/>
       <c r="G90" s="24"/>
-      <c r="H90" s="24"/>
+      <c r="H90" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I90" s="59" t="s">
         <v>21</v>
       </c>
@@ -8303,7 +8402,9 @@
       <c r="E91" s="25"/>
       <c r="F91" s="25"/>
       <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
+      <c r="H91" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I91" s="59" t="s">
         <v>21</v>
       </c>
@@ -8342,7 +8443,9 @@
       <c r="E92" s="25"/>
       <c r="F92" s="25"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="25"/>
+      <c r="H92" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I92" s="59" t="s">
         <v>21</v>
       </c>
@@ -8382,7 +8485,9 @@
       <c r="E93" s="24"/>
       <c r="F93" s="24"/>
       <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
+      <c r="H93" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I93" s="59" t="s">
         <v>21</v>
       </c>
@@ -8422,7 +8527,9 @@
       <c r="E94" s="24"/>
       <c r="F94" s="24"/>
       <c r="G94" s="24"/>
-      <c r="H94" s="24"/>
+      <c r="H94" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I94" s="59" t="s">
         <v>21</v>
       </c>
@@ -8460,7 +8567,9 @@
       <c r="E95" s="24"/>
       <c r="F95" s="24"/>
       <c r="G95" s="24"/>
-      <c r="H95" s="24"/>
+      <c r="H95" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I95" s="59" t="s">
         <v>21</v>
       </c>
@@ -8498,7 +8607,9 @@
       <c r="E96" s="24"/>
       <c r="F96" s="24"/>
       <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
+      <c r="H96" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I96" s="59" t="s">
         <v>21</v>
       </c>
@@ -8536,7 +8647,9 @@
       <c r="E97" s="24"/>
       <c r="F97" s="24"/>
       <c r="G97" s="24"/>
-      <c r="H97" s="24"/>
+      <c r="H97" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I97" s="59" t="s">
         <v>21</v>
       </c>
@@ -8574,7 +8687,9 @@
       <c r="E98" s="24"/>
       <c r="F98" s="24"/>
       <c r="G98" s="24"/>
-      <c r="H98" s="24"/>
+      <c r="H98" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I98" s="59" t="s">
         <v>21</v>
       </c>
@@ -8612,7 +8727,9 @@
       <c r="E99" s="24"/>
       <c r="F99" s="24"/>
       <c r="G99" s="24"/>
-      <c r="H99" s="24"/>
+      <c r="H99" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I99" s="59" t="s">
         <v>21</v>
       </c>
@@ -8650,7 +8767,9 @@
       <c r="E100" s="24"/>
       <c r="F100" s="24"/>
       <c r="G100" s="24"/>
-      <c r="H100" s="24"/>
+      <c r="H100" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I100" s="59" t="s">
         <v>21</v>
       </c>
@@ -8688,7 +8807,9 @@
       <c r="E101" s="24"/>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
+      <c r="H101" s="61" t="s">
+        <v>1158</v>
+      </c>
       <c r="I101" s="59" t="s">
         <v>21</v>
       </c>
@@ -9341,7 +9462,9 @@
       <c r="E118" s="42"/>
       <c r="F118" s="42"/>
       <c r="G118" s="24"/>
-      <c r="H118" s="39"/>
+      <c r="H118" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I118" s="59" t="s">
         <v>22</v>
       </c>
@@ -9379,7 +9502,9 @@
       <c r="E119" s="42"/>
       <c r="F119" s="42"/>
       <c r="G119" s="24"/>
-      <c r="H119" s="39"/>
+      <c r="H119" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I119" s="59" t="s">
         <v>22</v>
       </c>
@@ -9419,7 +9544,9 @@
       <c r="E120" s="24"/>
       <c r="F120" s="24"/>
       <c r="G120" s="24"/>
-      <c r="H120" s="24"/>
+      <c r="H120" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I120" s="59" t="s">
         <v>22</v>
       </c>
@@ -9457,7 +9584,9 @@
       <c r="E121" s="24"/>
       <c r="F121" s="24"/>
       <c r="G121" s="24"/>
-      <c r="H121" s="24"/>
+      <c r="H121" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I121" s="59" t="s">
         <v>22</v>
       </c>
@@ -9495,7 +9624,9 @@
       <c r="E122" s="24"/>
       <c r="F122" s="24"/>
       <c r="G122" s="24"/>
-      <c r="H122" s="24"/>
+      <c r="H122" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I122" s="59" t="s">
         <v>22</v>
       </c>
@@ -9533,7 +9664,9 @@
       <c r="E123" s="24"/>
       <c r="F123" s="24"/>
       <c r="G123" s="24"/>
-      <c r="H123" s="24"/>
+      <c r="H123" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I123" s="59" t="s">
         <v>22</v>
       </c>
@@ -9571,7 +9704,9 @@
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
       <c r="G124" s="24"/>
-      <c r="H124" s="24"/>
+      <c r="H124" s="61" t="s">
+        <v>1160</v>
+      </c>
       <c r="I124" s="59" t="s">
         <v>22</v>
       </c>
@@ -10453,7 +10588,9 @@
       <c r="E147" s="24"/>
       <c r="F147" s="24"/>
       <c r="G147" s="24"/>
-      <c r="H147" s="24"/>
+      <c r="H147" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I147" s="59" t="s">
         <v>22</v>
       </c>
@@ -10491,7 +10628,9 @@
       <c r="E148" s="24"/>
       <c r="F148" s="24"/>
       <c r="G148" s="24"/>
-      <c r="H148" s="24"/>
+      <c r="H148" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I148" s="59" t="s">
         <v>22</v>
       </c>
@@ -10528,7 +10667,9 @@
       <c r="E149" s="24"/>
       <c r="F149" s="24"/>
       <c r="G149" s="42"/>
-      <c r="H149" s="24"/>
+      <c r="H149" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I149" s="59" t="s">
         <v>22</v>
       </c>
@@ -10566,7 +10707,9 @@
       <c r="E150" s="24"/>
       <c r="F150" s="24"/>
       <c r="G150" s="42"/>
-      <c r="H150" s="24"/>
+      <c r="H150" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I150" s="59" t="s">
         <v>22</v>
       </c>
@@ -10604,7 +10747,9 @@
       <c r="E151" s="24"/>
       <c r="F151" s="24"/>
       <c r="G151" s="42"/>
-      <c r="H151" s="24"/>
+      <c r="H151" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I151" s="59" t="s">
         <v>22</v>
       </c>
@@ -10642,7 +10787,9 @@
       <c r="E152" s="24"/>
       <c r="F152" s="24"/>
       <c r="G152" s="24"/>
-      <c r="H152" s="24"/>
+      <c r="H152" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I152" s="59" t="s">
         <v>23</v>
       </c>
@@ -10679,7 +10826,9 @@
       <c r="E153" s="24"/>
       <c r="F153" s="24"/>
       <c r="G153" s="24"/>
-      <c r="H153" s="24"/>
+      <c r="H153" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I153" s="59" t="s">
         <v>23</v>
       </c>
@@ -10717,7 +10866,9 @@
       <c r="E154" s="24"/>
       <c r="F154" s="24"/>
       <c r="G154" s="24"/>
-      <c r="H154" s="24"/>
+      <c r="H154" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I154" s="59" t="s">
         <v>23</v>
       </c>
@@ -10755,7 +10906,9 @@
       <c r="E155" s="24"/>
       <c r="F155" s="24"/>
       <c r="G155" s="24"/>
-      <c r="H155" s="24"/>
+      <c r="H155" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I155" s="59" t="s">
         <v>23</v>
       </c>
@@ -10795,7 +10948,9 @@
       <c r="E156" s="24"/>
       <c r="F156" s="24"/>
       <c r="G156" s="24"/>
-      <c r="H156" s="24"/>
+      <c r="H156" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I156" s="59" t="s">
         <v>23</v>
       </c>
@@ -10833,7 +10988,9 @@
       <c r="E157" s="24"/>
       <c r="F157" s="24"/>
       <c r="G157" s="24"/>
-      <c r="H157" s="24"/>
+      <c r="H157" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I157" s="59" t="s">
         <v>23</v>
       </c>
@@ -10871,7 +11028,9 @@
       <c r="E158" s="24"/>
       <c r="F158" s="24"/>
       <c r="G158" s="24"/>
-      <c r="H158" s="24"/>
+      <c r="H158" s="61" t="s">
+        <v>1161</v>
+      </c>
       <c r="I158" s="59" t="s">
         <v>23</v>
       </c>
@@ -11255,7 +11414,9 @@
       <c r="E168" s="24"/>
       <c r="F168" s="24"/>
       <c r="G168" s="24"/>
-      <c r="H168" s="24"/>
+      <c r="H168" s="61" t="s">
+        <v>1162</v>
+      </c>
       <c r="I168" s="59" t="s">
         <v>23</v>
       </c>
@@ -11293,7 +11454,9 @@
       <c r="E169" s="24"/>
       <c r="F169" s="24"/>
       <c r="G169" s="24"/>
-      <c r="H169" s="24"/>
+      <c r="H169" s="61" t="s">
+        <v>1162</v>
+      </c>
       <c r="I169" s="59" t="s">
         <v>23</v>
       </c>
@@ -11333,7 +11496,9 @@
       <c r="E170" s="24"/>
       <c r="F170" s="24"/>
       <c r="G170" s="24"/>
-      <c r="H170" s="24"/>
+      <c r="H170" s="61" t="s">
+        <v>1162</v>
+      </c>
       <c r="I170" s="59" t="s">
         <v>23</v>
       </c>
@@ -11371,7 +11536,9 @@
       <c r="E171" s="24"/>
       <c r="F171" s="24"/>
       <c r="G171" s="24"/>
-      <c r="H171" s="24"/>
+      <c r="H171" s="61" t="s">
+        <v>1162</v>
+      </c>
       <c r="I171" s="59" t="s">
         <v>23</v>
       </c>
@@ -12065,7 +12232,9 @@
       <c r="E189" s="24"/>
       <c r="F189" s="24"/>
       <c r="G189" s="24"/>
-      <c r="H189" s="24"/>
+      <c r="H189" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I189" s="59" t="s">
         <v>23</v>
       </c>
@@ -12103,7 +12272,9 @@
       <c r="E190" s="24"/>
       <c r="F190" s="24"/>
       <c r="G190" s="24"/>
-      <c r="H190" s="24"/>
+      <c r="H190" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I190" s="59" t="s">
         <v>23</v>
       </c>
@@ -12141,7 +12312,9 @@
       <c r="E191" s="24"/>
       <c r="F191" s="24"/>
       <c r="G191" s="24"/>
-      <c r="H191" s="24"/>
+      <c r="H191" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I191" s="59" t="s">
         <v>23</v>
       </c>
@@ -12179,7 +12352,9 @@
       <c r="E192" s="24"/>
       <c r="F192" s="24"/>
       <c r="G192" s="24"/>
-      <c r="H192" s="24"/>
+      <c r="H192" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I192" s="59" t="s">
         <v>23</v>
       </c>
@@ -12217,7 +12392,9 @@
       <c r="E193" s="24"/>
       <c r="F193" s="24"/>
       <c r="G193" s="24"/>
-      <c r="H193" s="24"/>
+      <c r="H193" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I193" s="59" t="s">
         <v>23</v>
       </c>
@@ -12255,7 +12432,9 @@
       <c r="E194" s="24"/>
       <c r="F194" s="24"/>
       <c r="G194" s="24"/>
-      <c r="H194" s="24"/>
+      <c r="H194" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I194" s="59" t="s">
         <v>23</v>
       </c>
@@ -12293,7 +12472,9 @@
       <c r="E195" s="24"/>
       <c r="F195" s="24"/>
       <c r="G195" s="24"/>
-      <c r="H195" s="24"/>
+      <c r="H195" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I195" s="59" t="s">
         <v>23</v>
       </c>
@@ -12331,7 +12512,9 @@
       <c r="E196" s="24"/>
       <c r="F196" s="24"/>
       <c r="G196" s="24"/>
-      <c r="H196" s="24"/>
+      <c r="H196" s="61" t="s">
+        <v>1163</v>
+      </c>
       <c r="I196" s="59" t="s">
         <v>23</v>
       </c>
@@ -13446,7 +13629,9 @@
       <c r="E225" s="24"/>
       <c r="F225" s="24"/>
       <c r="G225" s="24"/>
-      <c r="H225" s="24"/>
+      <c r="H225" s="61" t="s">
+        <v>1167</v>
+      </c>
       <c r="I225" s="59" t="s">
         <v>24</v>
       </c>
@@ -13472,8 +13657,12 @@
       <c r="P225" s="8"/>
       <c r="Q225" s="8"/>
       <c r="R225" s="8"/>
-      <c r="S225" s="8"/>
-      <c r="T225" s="8"/>
+      <c r="S225" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="T225" s="8" t="s">
+        <v>1168</v>
+      </c>
       <c r="U225" s="8"/>
       <c r="V225" s="56" t="s">
         <v>183</v>
@@ -13484,7 +13673,9 @@
       <c r="E226" s="24"/>
       <c r="F226" s="24"/>
       <c r="G226" s="24"/>
-      <c r="H226" s="24"/>
+      <c r="H226" s="61" t="s">
+        <v>1167</v>
+      </c>
       <c r="I226" s="59" t="s">
         <v>24</v>
       </c>
@@ -13522,7 +13713,9 @@
       <c r="E227" s="24"/>
       <c r="F227" s="24"/>
       <c r="G227" s="24"/>
-      <c r="H227" s="24"/>
+      <c r="H227" s="61" t="s">
+        <v>1167</v>
+      </c>
       <c r="I227" s="59" t="s">
         <v>24</v>
       </c>
@@ -13560,7 +13753,9 @@
       <c r="E228" s="24"/>
       <c r="F228" s="24"/>
       <c r="G228" s="24"/>
-      <c r="H228" s="24"/>
+      <c r="H228" s="61" t="s">
+        <v>1167</v>
+      </c>
       <c r="I228" s="59" t="s">
         <v>24</v>
       </c>
@@ -13712,7 +13907,9 @@
       <c r="E232" s="24"/>
       <c r="F232" s="24"/>
       <c r="G232" s="24"/>
-      <c r="H232" s="24"/>
+      <c r="H232" s="61" t="s">
+        <v>1164</v>
+      </c>
       <c r="I232" s="59" t="s">
         <v>24</v>
       </c>
@@ -13752,7 +13949,9 @@
       <c r="E233" s="24"/>
       <c r="F233" s="24"/>
       <c r="G233" s="24"/>
-      <c r="H233" s="24"/>
+      <c r="H233" s="61" t="s">
+        <v>1164</v>
+      </c>
       <c r="I233" s="59" t="s">
         <v>24</v>
       </c>
@@ -13778,8 +13977,12 @@
       <c r="P233" s="8"/>
       <c r="Q233" s="8"/>
       <c r="R233" s="8"/>
-      <c r="S233" s="8"/>
-      <c r="T233" s="8"/>
+      <c r="S233" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="T233" s="8" t="s">
+        <v>1166</v>
+      </c>
       <c r="U233" s="8"/>
       <c r="V233" s="56" t="s">
         <v>188</v>
@@ -13790,7 +13993,9 @@
       <c r="E234" s="24"/>
       <c r="F234" s="24"/>
       <c r="G234" s="24"/>
-      <c r="H234" s="24"/>
+      <c r="H234" s="61" t="s">
+        <v>1164</v>
+      </c>
       <c r="I234" s="59" t="s">
         <v>24</v>
       </c>
@@ -15210,7 +15415,9 @@
       <c r="E271" s="24"/>
       <c r="F271" s="24"/>
       <c r="G271" s="24"/>
-      <c r="H271" s="24"/>
+      <c r="H271" s="61" t="s">
+        <v>1169</v>
+      </c>
       <c r="I271" s="59" t="s">
         <v>25</v>
       </c>
@@ -15248,7 +15455,9 @@
       <c r="E272" s="24"/>
       <c r="F272" s="24"/>
       <c r="G272" s="24"/>
-      <c r="H272" s="24"/>
+      <c r="H272" s="61" t="s">
+        <v>1169</v>
+      </c>
       <c r="I272" s="59" t="s">
         <v>25</v>
       </c>
@@ -15286,7 +15495,9 @@
       <c r="E273" s="24"/>
       <c r="F273" s="24"/>
       <c r="G273" s="24"/>
-      <c r="H273" s="24"/>
+      <c r="H273" s="61" t="s">
+        <v>1169</v>
+      </c>
       <c r="I273" s="59" t="s">
         <v>25</v>
       </c>
@@ -15324,7 +15535,9 @@
       <c r="E274" s="24"/>
       <c r="F274" s="24"/>
       <c r="G274" s="24"/>
-      <c r="H274" s="24"/>
+      <c r="H274" s="61" t="s">
+        <v>1169</v>
+      </c>
       <c r="I274" s="59" t="s">
         <v>25</v>
       </c>
@@ -31718,7 +31931,9 @@
       <c r="E702" s="24"/>
       <c r="F702" s="24"/>
       <c r="G702" s="24"/>
-      <c r="H702" s="24"/>
+      <c r="H702" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I702" s="59" t="s">
         <v>34</v>
       </c>
@@ -31754,7 +31969,9 @@
       <c r="E703" s="24"/>
       <c r="F703" s="24"/>
       <c r="G703" s="24"/>
-      <c r="H703" s="24"/>
+      <c r="H703" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I703" s="59" t="s">
         <v>34</v>
       </c>
@@ -31791,7 +32008,9 @@
       <c r="E704" s="24"/>
       <c r="F704" s="24"/>
       <c r="G704" s="24"/>
-      <c r="H704" s="24"/>
+      <c r="H704" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I704" s="59" t="s">
         <v>34</v>
       </c>
@@ -31824,11 +32043,16 @@
         <v>245</v>
       </c>
     </row>
-    <row r="705" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A705" s="2" t="s">
+        <v>1171</v>
+      </c>
       <c r="E705" s="24"/>
       <c r="F705" s="24"/>
       <c r="G705" s="24"/>
-      <c r="H705" s="24"/>
+      <c r="H705" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I705" s="59" t="s">
         <v>34</v>
       </c>
@@ -31861,11 +32085,16 @@
         <v>385</v>
       </c>
     </row>
-    <row r="706" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A706" s="2" t="s">
+        <v>1171</v>
+      </c>
       <c r="E706" s="24"/>
       <c r="F706" s="24"/>
       <c r="G706" s="24"/>
-      <c r="H706" s="24"/>
+      <c r="H706" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I706" s="59" t="s">
         <v>34</v>
       </c>
@@ -31898,11 +32127,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="707" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A707" s="2" t="s">
+        <v>1171</v>
+      </c>
       <c r="E707" s="24"/>
       <c r="F707" s="24"/>
       <c r="G707" s="24"/>
-      <c r="H707" s="24"/>
+      <c r="H707" s="61" t="s">
+        <v>1170</v>
+      </c>
       <c r="I707" s="59" t="s">
         <v>34</v>
       </c>
@@ -31935,7 +32169,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="708" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E708" s="24"/>
       <c r="F708" s="24"/>
       <c r="G708" s="24"/>
@@ -31972,7 +32206,7 @@
       <c r="U708" s="8"/>
       <c r="V708" s="56"/>
     </row>
-    <row r="709" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E709" s="24"/>
       <c r="F709" s="24"/>
       <c r="G709" s="24"/>
@@ -32009,7 +32243,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="710" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E710" s="24"/>
       <c r="F710" s="24"/>
       <c r="G710" s="24"/>
@@ -32046,7 +32280,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="711" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E711" s="24"/>
       <c r="F711" s="24"/>
       <c r="G711" s="24"/>
@@ -32083,7 +32317,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="712" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E712" s="24"/>
       <c r="F712" s="24"/>
       <c r="G712" s="24"/>
@@ -32120,7 +32354,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="713" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E713" s="24"/>
       <c r="F713" s="24"/>
       <c r="G713" s="24"/>
@@ -32157,7 +32391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="714" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E714" s="24"/>
       <c r="F714" s="24"/>
       <c r="G714" s="24"/>
@@ -32196,7 +32430,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="715" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E715" s="24"/>
       <c r="F715" s="24"/>
       <c r="G715" s="24"/>
@@ -32233,7 +32467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="716" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E716" s="24"/>
       <c r="F716" s="24"/>
       <c r="G716" s="24"/>
@@ -32272,7 +32506,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="717" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="D717" s="48"/>
       <c r="E717" s="24"/>
       <c r="F717" s="24"/>
@@ -32310,7 +32544,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="718" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E718" s="24"/>
       <c r="F718" s="24"/>
       <c r="G718" s="24"/>
@@ -32347,7 +32581,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="719" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E719" s="24"/>
       <c r="F719" s="24"/>
       <c r="G719" s="24"/>
@@ -32384,7 +32618,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="720" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E720" s="24"/>
       <c r="F720" s="24"/>
       <c r="G720" s="24"/>
@@ -34595,7 +34829,9 @@
       <c r="E779" s="24"/>
       <c r="F779" s="24"/>
       <c r="G779" s="24"/>
-      <c r="H779" s="24"/>
+      <c r="H779" s="61" t="s">
+        <v>1172</v>
+      </c>
       <c r="I779" s="59" t="s">
         <v>35</v>
       </c>
@@ -34632,7 +34868,9 @@
       <c r="E780" s="24"/>
       <c r="F780" s="24"/>
       <c r="G780" s="24"/>
-      <c r="H780" s="24"/>
+      <c r="H780" s="61" t="s">
+        <v>1172</v>
+      </c>
       <c r="I780" s="59" t="s">
         <v>35</v>
       </c>
@@ -34660,8 +34898,12 @@
       <c r="P780" s="8"/>
       <c r="Q780" s="8"/>
       <c r="R780" s="8"/>
-      <c r="S780" s="8"/>
-      <c r="T780" s="8"/>
+      <c r="S780" s="8" t="s">
+        <v>1173</v>
+      </c>
+      <c r="T780" s="8" t="s">
+        <v>1174</v>
+      </c>
       <c r="U780" s="8"/>
       <c r="V780" s="56"/>
     </row>
@@ -34669,7 +34911,9 @@
       <c r="E781" s="24"/>
       <c r="F781" s="24"/>
       <c r="G781" s="24"/>
-      <c r="H781" s="24"/>
+      <c r="H781" s="61" t="s">
+        <v>1172</v>
+      </c>
       <c r="I781" s="59" t="s">
         <v>35</v>
       </c>
@@ -39890,7 +40134,9 @@
       <c r="E920" s="24"/>
       <c r="F920" s="24"/>
       <c r="G920" s="24"/>
-      <c r="H920" s="24"/>
+      <c r="H920" s="61" t="s">
+        <v>1175</v>
+      </c>
       <c r="I920" s="59" t="s">
         <v>38</v>
       </c>
@@ -39927,7 +40173,9 @@
       <c r="E921" s="24"/>
       <c r="F921" s="24"/>
       <c r="G921" s="24"/>
-      <c r="H921" s="24"/>
+      <c r="H921" s="61" t="s">
+        <v>1175</v>
+      </c>
       <c r="I921" s="59" t="s">
         <v>38</v>
       </c>
@@ -39964,7 +40212,9 @@
       <c r="E922" s="24"/>
       <c r="F922" s="24"/>
       <c r="G922" s="24"/>
-      <c r="H922" s="24"/>
+      <c r="H922" s="61" t="s">
+        <v>1175</v>
+      </c>
       <c r="I922" s="59" t="s">
         <v>38</v>
       </c>
@@ -40001,7 +40251,9 @@
       <c r="E923" s="24"/>
       <c r="F923" s="24"/>
       <c r="G923" s="24"/>
-      <c r="H923" s="24"/>
+      <c r="H923" s="61" t="s">
+        <v>1175</v>
+      </c>
       <c r="I923" s="59" t="s">
         <v>38</v>
       </c>
@@ -40038,7 +40290,9 @@
       <c r="E924" s="24"/>
       <c r="F924" s="24"/>
       <c r="G924" s="24"/>
-      <c r="H924" s="24"/>
+      <c r="H924" s="61" t="s">
+        <v>1175</v>
+      </c>
       <c r="I924" s="59" t="s">
         <v>38</v>
       </c>
@@ -53630,7 +53884,9 @@
       <c r="E1287" s="24"/>
       <c r="F1287" s="24"/>
       <c r="G1287" s="24"/>
-      <c r="H1287" s="24"/>
+      <c r="H1287" s="61" t="s">
+        <v>1176</v>
+      </c>
       <c r="I1287" s="59" t="s">
         <v>45</v>
       </c>
@@ -53667,7 +53923,9 @@
       <c r="E1288" s="24"/>
       <c r="F1288" s="24"/>
       <c r="G1288" s="24"/>
-      <c r="H1288" s="24"/>
+      <c r="H1288" s="61" t="s">
+        <v>1176</v>
+      </c>
       <c r="I1288" s="59" t="s">
         <v>45</v>
       </c>
@@ -53704,7 +53962,9 @@
       <c r="E1289" s="24"/>
       <c r="F1289" s="24"/>
       <c r="G1289" s="24"/>
-      <c r="H1289" s="24"/>
+      <c r="H1289" s="61" t="s">
+        <v>1176</v>
+      </c>
       <c r="I1289" s="59" t="s">
         <v>45</v>
       </c>
@@ -53743,7 +54003,9 @@
       <c r="E1290" s="24"/>
       <c r="F1290" s="24"/>
       <c r="G1290" s="24"/>
-      <c r="H1290" s="24"/>
+      <c r="H1290" s="61" t="s">
+        <v>1176</v>
+      </c>
       <c r="I1290" s="59" t="s">
         <v>45</v>
       </c>
@@ -53771,8 +54033,12 @@
       <c r="P1290" s="8"/>
       <c r="Q1290" s="8"/>
       <c r="R1290" s="8"/>
-      <c r="S1290" s="8"/>
-      <c r="T1290" s="8"/>
+      <c r="S1290" s="8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="T1290" s="8" t="s">
+        <v>1174</v>
+      </c>
       <c r="U1290" s="8"/>
       <c r="V1290" s="56"/>
     </row>
@@ -53780,7 +54046,9 @@
       <c r="E1291" s="24"/>
       <c r="F1291" s="24"/>
       <c r="G1291" s="24"/>
-      <c r="H1291" s="24"/>
+      <c r="H1291" s="61" t="s">
+        <v>1176</v>
+      </c>
       <c r="I1291" s="59" t="s">
         <v>45</v>
       </c>
@@ -65385,7 +65653,10 @@
         <v>611</v>
       </c>
     </row>
-    <row r="1601" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1601" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1601" s="61" t="s">
+        <v>1178</v>
+      </c>
       <c r="I1601" s="59" t="s">
         <v>51</v>
       </c>
@@ -65411,7 +65682,10 @@
         <v>612</v>
       </c>
     </row>
-    <row r="1602" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1602" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1602" s="61" t="s">
+        <v>1178</v>
+      </c>
       <c r="I1602" s="59" t="s">
         <v>51</v>
       </c>
@@ -65437,7 +65711,10 @@
         <v>613</v>
       </c>
     </row>
-    <row r="1603" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1603" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1603" s="61" t="s">
+        <v>1178</v>
+      </c>
       <c r="I1603" s="59" t="s">
         <v>51</v>
       </c>
@@ -65464,7 +65741,10 @@
       </c>
       <c r="V1603" s="56"/>
     </row>
-    <row r="1604" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1604" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1604" s="61" t="s">
+        <v>1178</v>
+      </c>
       <c r="I1604" s="59" t="s">
         <v>51</v>
       </c>
@@ -65490,7 +65770,10 @@
         <v>614</v>
       </c>
     </row>
-    <row r="1605" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1605" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1605" s="61" t="s">
+        <v>1178</v>
+      </c>
       <c r="I1605" s="59" t="s">
         <v>51</v>
       </c>
@@ -65519,7 +65802,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="1606" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1606" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1606" s="59" t="s">
         <v>51</v>
       </c>
@@ -65545,7 +65828,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="1607" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1607" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1607" s="59" t="s">
         <v>51</v>
       </c>
@@ -65574,7 +65857,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="1608" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1608" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1608" s="59" t="s">
         <v>51</v>
       </c>
@@ -65601,7 +65884,7 @@
       </c>
       <c r="V1608" s="56"/>
     </row>
-    <row r="1609" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1609" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1609" s="59" t="s">
         <v>51</v>
       </c>
@@ -65627,7 +65910,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="1610" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1610" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1610" s="59" t="s">
         <v>51</v>
       </c>
@@ -65653,7 +65936,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="1611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1611" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1611" s="59" t="s">
         <v>51</v>
       </c>
@@ -65679,7 +65962,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="1612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1612" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1612" s="59" t="s">
         <v>51</v>
       </c>
@@ -65705,7 +65988,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="1613" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1613" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1613" s="59" t="s">
         <v>51</v>
       </c>
@@ -65734,7 +66017,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="1614" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1614" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1614" s="59" t="s">
         <v>51</v>
       </c>
@@ -65763,7 +66046,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="1615" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1615" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1615" s="59" t="s">
         <v>51</v>
       </c>
@@ -65789,7 +66072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="1616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1616" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1616" s="59" t="s">
         <v>51</v>
       </c>
@@ -67073,7 +67356,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="1665" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1665" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1665" s="59" t="s">
         <v>52</v>
       </c>
@@ -67099,7 +67382,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="1666" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1666" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1666" s="59" t="s">
         <v>52</v>
       </c>
@@ -67125,7 +67408,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="1667" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1667" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1667" s="59" t="s">
         <v>52</v>
       </c>
@@ -67151,7 +67434,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="1668" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1668" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1668" s="59" t="s">
         <v>52</v>
       </c>
@@ -67177,7 +67460,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="1669" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1669" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1669" s="59" t="s">
         <v>52</v>
       </c>
@@ -67203,7 +67486,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="1670" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1670" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1670" s="59" t="s">
         <v>52</v>
       </c>
@@ -67229,7 +67512,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="1671" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1671" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1671" s="59" t="s">
         <v>52</v>
       </c>
@@ -67258,7 +67541,10 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="1672" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1672" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1672" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1672" s="59" t="s">
         <v>53</v>
       </c>
@@ -67283,7 +67569,10 @@
       </c>
       <c r="V1672" s="56"/>
     </row>
-    <row r="1673" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1673" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1673" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1673" s="59" t="s">
         <v>53</v>
       </c>
@@ -67309,7 +67598,10 @@
         <v>646</v>
       </c>
     </row>
-    <row r="1674" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1674" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1674" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1674" s="59" t="s">
         <v>53</v>
       </c>
@@ -67335,7 +67627,10 @@
         <v>647</v>
       </c>
     </row>
-    <row r="1675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1675" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1675" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1675" s="59" t="s">
         <v>53</v>
       </c>
@@ -67361,7 +67656,10 @@
         <v>648</v>
       </c>
     </row>
-    <row r="1676" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1676" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1676" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1676" s="59" t="s">
         <v>53</v>
       </c>
@@ -67388,7 +67686,10 @@
       </c>
       <c r="V1676" s="56"/>
     </row>
-    <row r="1677" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1677" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1677" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1677" s="59" t="s">
         <v>53</v>
       </c>
@@ -67417,7 +67718,10 @@
         <v>649</v>
       </c>
     </row>
-    <row r="1678" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1678" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1678" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1678" s="59" t="s">
         <v>53</v>
       </c>
@@ -67443,7 +67747,10 @@
         <v>646</v>
       </c>
     </row>
-    <row r="1679" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1679" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1679" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1679" s="59" t="s">
         <v>53</v>
       </c>
@@ -67470,7 +67777,10 @@
       </c>
       <c r="V1679" s="56"/>
     </row>
-    <row r="1680" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1680" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1680" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1680" s="59" t="s">
         <v>53</v>
       </c>
@@ -67496,7 +67806,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1681" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1681" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1681" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1681" s="59" t="s">
         <v>53</v>
       </c>
@@ -67522,7 +67835,10 @@
         <v>450</v>
       </c>
     </row>
-    <row r="1682" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1682" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1682" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1682" s="59" t="s">
         <v>53</v>
       </c>
@@ -67548,7 +67864,10 @@
         <v>651</v>
       </c>
     </row>
-    <row r="1683" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1683" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1683" s="61" t="s">
+        <v>1179</v>
+      </c>
       <c r="I1683" s="59" t="s">
         <v>53</v>
       </c>
@@ -67580,7 +67899,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="1684" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1684" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1684" s="59" t="s">
         <v>53</v>
       </c>
@@ -67606,7 +67925,10 @@
         <v>653</v>
       </c>
     </row>
-    <row r="1685" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1685" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1685" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1685" s="59" t="s">
         <v>53</v>
       </c>
@@ -67632,7 +67954,10 @@
         <v>654</v>
       </c>
     </row>
-    <row r="1686" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1686" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1686" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1686" s="59" t="s">
         <v>53</v>
       </c>
@@ -67658,7 +67983,10 @@
         <v>655</v>
       </c>
     </row>
-    <row r="1687" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1687" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1687" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1687" s="59" t="s">
         <v>53</v>
       </c>
@@ -67684,7 +68012,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1688" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1688" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1688" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1688" s="59" t="s">
         <v>53</v>
       </c>
@@ -67711,7 +68042,10 @@
       </c>
       <c r="V1688" s="56"/>
     </row>
-    <row r="1689" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1689" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1689" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1689" s="59" t="s">
         <v>53</v>
       </c>
@@ -67737,7 +68071,10 @@
         <v>656</v>
       </c>
     </row>
-    <row r="1690" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1690" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1690" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1690" s="59" t="s">
         <v>53</v>
       </c>
@@ -67763,7 +68100,10 @@
         <v>657</v>
       </c>
     </row>
-    <row r="1691" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1691" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1691" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1691" s="59" t="s">
         <v>53</v>
       </c>
@@ -67789,7 +68129,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1692" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1692" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1692" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1692" s="59" t="s">
         <v>53</v>
       </c>
@@ -67815,7 +68158,10 @@
         <v>658</v>
       </c>
     </row>
-    <row r="1693" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1693" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1693" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1693" s="59" t="s">
         <v>53</v>
       </c>
@@ -67841,7 +68187,10 @@
         <v>659</v>
       </c>
     </row>
-    <row r="1694" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1694" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1694" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1694" s="59" t="s">
         <v>53</v>
       </c>
@@ -67868,7 +68217,10 @@
       </c>
       <c r="V1694" s="56"/>
     </row>
-    <row r="1695" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1695" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1695" s="61" t="s">
+        <v>1180</v>
+      </c>
       <c r="I1695" s="59" t="s">
         <v>53</v>
       </c>
@@ -67897,7 +68249,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="1696" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1696" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1696" s="59" t="s">
         <v>53</v>
       </c>
@@ -68354,7 +68706,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="1713" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1713" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1713" s="59" t="s">
         <v>53</v>
       </c>
@@ -68380,7 +68732,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1714" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1714" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1714" s="59" t="s">
         <v>53</v>
       </c>
@@ -68406,7 +68758,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="1715" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1715" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1715" s="59" t="s">
         <v>53</v>
       </c>
@@ -68432,7 +68784,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="1716" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1716" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1716" s="59" t="s">
         <v>53</v>
       </c>
@@ -68459,7 +68811,7 @@
       </c>
       <c r="V1716" s="56"/>
     </row>
-    <row r="1717" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1717" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1717" s="59" t="s">
         <v>53</v>
       </c>
@@ -68488,7 +68840,10 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="1718" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1718" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1718" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1718" s="59" t="s">
         <v>53</v>
       </c>
@@ -68515,7 +68870,10 @@
       </c>
       <c r="V1718" s="56"/>
     </row>
-    <row r="1719" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1719" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1719" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1719" s="59" t="s">
         <v>53</v>
       </c>
@@ -68541,7 +68899,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1720" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1720" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1720" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1720" s="59" t="s">
         <v>53</v>
       </c>
@@ -68570,7 +68931,10 @@
         <v>669</v>
       </c>
     </row>
-    <row r="1721" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1721" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1721" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1721" s="59" t="s">
         <v>53</v>
       </c>
@@ -68596,7 +68960,10 @@
         <v>651</v>
       </c>
     </row>
-    <row r="1722" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1722" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1722" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1722" s="59" t="s">
         <v>53</v>
       </c>
@@ -68622,7 +68989,10 @@
         <v>670</v>
       </c>
     </row>
-    <row r="1723" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1723" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1723" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1723" s="59" t="s">
         <v>53</v>
       </c>
@@ -68648,7 +69018,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="1724" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1724" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1724" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1724" s="59" t="s">
         <v>53</v>
       </c>
@@ -68677,7 +69050,10 @@
         <v>236</v>
       </c>
     </row>
-    <row r="1725" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1725" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1725" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1725" s="59" t="s">
         <v>53</v>
       </c>
@@ -68703,7 +69079,10 @@
         <v>650</v>
       </c>
     </row>
-    <row r="1726" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1726" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1726" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1726" s="59" t="s">
         <v>53</v>
       </c>
@@ -68730,7 +69109,10 @@
       </c>
       <c r="V1726" s="56"/>
     </row>
-    <row r="1727" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1727" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1727" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1727" s="59" t="s">
         <v>53</v>
       </c>
@@ -68756,7 +69138,10 @@
         <v>651</v>
       </c>
     </row>
-    <row r="1728" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1728" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1728" s="61" t="s">
+        <v>1181</v>
+      </c>
       <c r="I1728" s="59" t="s">
         <v>53</v>
       </c>
@@ -69633,7 +70018,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="1761" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1761" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1761" s="59" t="s">
         <v>54</v>
       </c>
@@ -69659,7 +70044,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="1762" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1762" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1762" s="59" t="s">
         <v>54</v>
       </c>
@@ -69685,7 +70070,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="1763" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1763" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1763" s="59" t="s">
         <v>54</v>
       </c>
@@ -69711,7 +70096,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="1764" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1764" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1764" s="59" t="s">
         <v>54</v>
       </c>
@@ -69737,7 +70122,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="1765" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1765" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1765" s="59" t="s">
         <v>54</v>
       </c>
@@ -69763,7 +70148,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="1766" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1766" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1766" s="59" t="s">
         <v>54</v>
       </c>
@@ -69789,7 +70174,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="1767" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1767" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1767" s="59" t="s">
         <v>54</v>
       </c>
@@ -69815,7 +70200,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="1768" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1768" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1768" s="59" t="s">
         <v>54</v>
       </c>
@@ -69841,7 +70226,10 @@
         <v>693</v>
       </c>
     </row>
-    <row r="1769" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1769" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1769" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1769" s="59" t="s">
         <v>54</v>
       </c>
@@ -69867,7 +70255,10 @@
         <v>694</v>
       </c>
     </row>
-    <row r="1770" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1770" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1770" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1770" s="59" t="s">
         <v>54</v>
       </c>
@@ -69893,7 +70284,10 @@
         <v>695</v>
       </c>
     </row>
-    <row r="1771" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1771" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1771" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1771" s="59" t="s">
         <v>54</v>
       </c>
@@ -69919,7 +70313,10 @@
         <v>696</v>
       </c>
     </row>
-    <row r="1772" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1772" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1772" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1772" s="59" t="s">
         <v>54</v>
       </c>
@@ -69945,7 +70342,10 @@
         <v>697</v>
       </c>
     </row>
-    <row r="1773" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1773" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1773" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1773" s="59" t="s">
         <v>54</v>
       </c>
@@ -69971,7 +70371,10 @@
         <v>698</v>
       </c>
     </row>
-    <row r="1774" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1774" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1774" s="61" t="s">
+        <v>1182</v>
+      </c>
       <c r="I1774" s="59" t="s">
         <v>54</v>
       </c>
@@ -69997,7 +70400,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="1775" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1775" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1775" s="59" t="s">
         <v>54</v>
       </c>
@@ -70023,7 +70426,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="1776" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1776" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1776" s="59" t="s">
         <v>54</v>
       </c>
@@ -70049,7 +70452,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="1777" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1777" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1777" s="59" t="s">
         <v>54</v>
       </c>
@@ -70075,7 +70478,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="1778" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1778" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1778" s="59" t="s">
         <v>54</v>
       </c>
@@ -70101,7 +70504,10 @@
         <v>703</v>
       </c>
     </row>
-    <row r="1779" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1779" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1779" s="61" t="s">
+        <v>1183</v>
+      </c>
       <c r="I1779" s="59" t="s">
         <v>54</v>
       </c>
@@ -70127,7 +70533,10 @@
         <v>704</v>
       </c>
     </row>
-    <row r="1780" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1780" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1780" s="61" t="s">
+        <v>1183</v>
+      </c>
       <c r="I1780" s="59" t="s">
         <v>54</v>
       </c>
@@ -70153,7 +70562,10 @@
         <v>705</v>
       </c>
     </row>
-    <row r="1781" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1781" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1781" s="61" t="s">
+        <v>1183</v>
+      </c>
       <c r="I1781" s="59" t="s">
         <v>54</v>
       </c>
@@ -70179,7 +70591,10 @@
         <v>706</v>
       </c>
     </row>
-    <row r="1782" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1782" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H1782" s="61" t="s">
+        <v>1183</v>
+      </c>
       <c r="I1782" s="59" t="s">
         <v>54</v>
       </c>
@@ -70205,7 +70620,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="1783" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1783" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1783" s="59" t="s">
         <v>54</v>
       </c>
@@ -70231,7 +70646,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="1784" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1784" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1784" s="59" t="s">
         <v>54</v>
       </c>
@@ -70257,7 +70672,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="1785" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1785" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1785" s="59" t="s">
         <v>54</v>
       </c>
@@ -70283,7 +70698,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="1786" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1786" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1786" s="59" t="s">
         <v>54</v>
       </c>
@@ -70309,7 +70724,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="1787" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1787" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1787" s="59" t="s">
         <v>54</v>
       </c>
@@ -70338,7 +70753,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="1788" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1788" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1788" s="59" t="s">
         <v>54</v>
       </c>
@@ -70364,7 +70779,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="1789" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1789" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1789" s="59" t="s">
         <v>54</v>
       </c>
@@ -70390,7 +70805,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="1790" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1790" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1790" s="59" t="s">
         <v>54</v>
       </c>
@@ -70419,7 +70834,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="1791" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1791" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1791" s="59" t="s">
         <v>55</v>
       </c>
@@ -70443,7 +70858,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="1792" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1792" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1792" s="59" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
TS 7.3 Padam template listening - 08/03/2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548B9912-8F33-42EC-B9C1-4E1C103174F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18936DC3-8B10-4212-8DE3-E4FF1056D9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5465" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="1182">
   <si>
     <t>Passage</t>
   </si>
@@ -3546,18 +3546,12 @@
     <t>RE?</t>
   </si>
   <si>
-    <t>SE?RE?</t>
-  </si>
-  <si>
     <t>N[S]</t>
   </si>
   <si>
     <t>P[S]+N[S]</t>
   </si>
   <si>
-    <t>SE,RE</t>
-  </si>
-  <si>
     <t>praqtya~g~g</t>
   </si>
   <si>
@@ -3577,6 +3571,9 @@
   </si>
   <si>
     <t>tiqro,a#hniyAH</t>
+  </si>
+  <si>
+    <t>P[c]</t>
   </si>
 </sst>
 </file>
@@ -3785,7 +3782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3957,6 +3954,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4241,10 +4241,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2728"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A743" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2124" sqref="N2124"/>
+      <selection pane="bottomLeft" activeCell="N746" sqref="N746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10277,9 +10277,7 @@
       <c r="R150" s="8"/>
       <c r="S150" s="8"/>
       <c r="T150" s="8"/>
-      <c r="U150" s="8" t="s">
-        <v>1171</v>
-      </c>
+      <c r="U150" s="8"/>
       <c r="V150" s="48"/>
     </row>
     <row r="151" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10315,9 +10313,7 @@
       <c r="R151" s="8"/>
       <c r="S151" s="8"/>
       <c r="T151" s="8"/>
-      <c r="U151" s="8" t="s">
-        <v>1170</v>
-      </c>
+      <c r="U151" s="8"/>
       <c r="V151" s="48"/>
     </row>
     <row r="152" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10793,9 +10789,7 @@
       <c r="R165" s="8"/>
       <c r="S165" s="8"/>
       <c r="T165" s="8"/>
-      <c r="U165" s="8" t="s">
-        <v>1170</v>
-      </c>
+      <c r="U165" s="8"/>
       <c r="V165" s="48" t="s">
         <v>908</v>
       </c>
@@ -10863,9 +10857,7 @@
       <c r="R167" s="8"/>
       <c r="S167" s="8"/>
       <c r="T167" s="8"/>
-      <c r="U167" s="8" t="s">
-        <v>1172</v>
-      </c>
+      <c r="U167" s="8"/>
       <c r="V167" s="48" t="s">
         <v>909</v>
       </c>
@@ -10976,9 +10968,7 @@
       <c r="R170" s="8"/>
       <c r="S170" s="8"/>
       <c r="T170" s="8"/>
-      <c r="U170" s="8" t="s">
-        <v>1171</v>
-      </c>
+      <c r="U170" s="8"/>
       <c r="V170" s="48"/>
     </row>
     <row r="171" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -11184,9 +11174,7 @@
       <c r="R176" s="8"/>
       <c r="S176" s="8"/>
       <c r="T176" s="8"/>
-      <c r="U176" s="8" t="s">
-        <v>1171</v>
-      </c>
+      <c r="U176" s="8"/>
       <c r="V176" s="48"/>
     </row>
     <row r="177" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -12297,9 +12285,7 @@
       <c r="R208" s="8"/>
       <c r="S208" s="8"/>
       <c r="T208" s="8"/>
-      <c r="U208" s="8" t="s">
-        <v>1170</v>
-      </c>
+      <c r="U208" s="8"/>
       <c r="V208" s="48"/>
     </row>
     <row r="209" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15126,7 +15112,7 @@
         <f t="shared" si="14"/>
         <v>91</v>
       </c>
-      <c r="N293" s="48" t="s">
+      <c r="N293" s="55" t="s">
         <v>214</v>
       </c>
       <c r="O293" s="7"/>
@@ -16967,8 +16953,12 @@
       <c r="P348" s="8"/>
       <c r="Q348" s="8"/>
       <c r="R348" s="8"/>
-      <c r="S348" s="8"/>
-      <c r="T348" s="8"/>
+      <c r="S348" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="T348" s="8" t="s">
+        <v>1181</v>
+      </c>
       <c r="U348" s="8"/>
       <c r="V348" s="48"/>
     </row>
@@ -17585,9 +17575,7 @@
       <c r="R366" s="8"/>
       <c r="S366" s="8"/>
       <c r="T366" s="8"/>
-      <c r="U366" s="8" t="s">
-        <v>1170</v>
-      </c>
+      <c r="U366" s="8"/>
       <c r="V366" s="48" t="s">
         <v>947</v>
       </c>
@@ -18252,7 +18240,7 @@
         <f t="shared" si="17"/>
         <v>93</v>
       </c>
-      <c r="N386" s="56" t="s">
+      <c r="N386" s="59" t="s">
         <v>281</v>
       </c>
       <c r="O386" s="7"/>
@@ -18975,7 +18963,7 @@
         <v>74</v>
       </c>
       <c r="T408" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="U408" s="8"/>
       <c r="V408" s="48"/>
@@ -19043,7 +19031,7 @@
         <v>74</v>
       </c>
       <c r="T410" s="8" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="U410" s="8"/>
       <c r="V410" s="48"/>
@@ -19403,7 +19391,7 @@
         <v>74</v>
       </c>
       <c r="T421" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="U421" s="8"/>
       <c r="V421" s="48"/>
@@ -19471,7 +19459,7 @@
         <v>74</v>
       </c>
       <c r="T423" s="8" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="U423" s="8"/>
       <c r="V423" s="48"/>
@@ -20951,9 +20939,7 @@
       <c r="R468" s="8"/>
       <c r="S468" s="8"/>
       <c r="T468" s="8"/>
-      <c r="U468" s="8" t="s">
-        <v>1175</v>
-      </c>
+      <c r="U468" s="8"/>
       <c r="V468" s="48"/>
     </row>
     <row r="469" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -21010,7 +20996,7 @@
         <f t="shared" si="23"/>
         <v>84</v>
       </c>
-      <c r="N470" s="48" t="s">
+      <c r="N470" s="55" t="s">
         <v>1133</v>
       </c>
       <c r="O470" s="8" t="s">
@@ -23060,7 +23046,7 @@
         <v>74</v>
       </c>
       <c r="T532" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="U532" s="8"/>
       <c r="V532" s="48"/>
@@ -23128,7 +23114,7 @@
         <v>74</v>
       </c>
       <c r="T534" s="8" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="U534" s="8"/>
       <c r="V534" s="48"/>
@@ -24042,9 +24028,7 @@
       <c r="R562" s="8"/>
       <c r="S562" s="8"/>
       <c r="T562" s="8"/>
-      <c r="U562" s="8" t="s">
-        <v>1170</v>
-      </c>
+      <c r="U562" s="8"/>
       <c r="V562" s="48"/>
     </row>
     <row r="563" spans="4:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -25624,9 +25608,7 @@
       <c r="R610" s="8"/>
       <c r="S610" s="8"/>
       <c r="T610" s="8"/>
-      <c r="U610" s="8" t="s">
-        <v>1171</v>
-      </c>
+      <c r="U610" s="8"/>
       <c r="V610" s="48" t="s">
         <v>962</v>
       </c>
@@ -25787,7 +25769,7 @@
         <v>145</v>
       </c>
       <c r="N615" s="57" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="O615" s="7"/>
       <c r="P615" s="8"/>
@@ -27100,7 +27082,7 @@
         <f t="shared" si="32"/>
         <v>3</v>
       </c>
-      <c r="N654" s="48" t="s">
+      <c r="N654" s="57" t="s">
         <v>1134</v>
       </c>
       <c r="O654" s="8" t="s">
@@ -30257,7 +30239,7 @@
         <f t="shared" si="35"/>
         <v>101</v>
       </c>
-      <c r="N752" s="48" t="s">
+      <c r="N752" s="55" t="s">
         <v>1133</v>
       </c>
       <c r="O752" s="8" t="s">
@@ -31188,7 +31170,7 @@
         <v>84</v>
       </c>
       <c r="T780" s="8" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="U780" s="8"/>
       <c r="V780" s="48"/>
@@ -31905,7 +31887,7 @@
         <v>84</v>
       </c>
       <c r="T802" s="8" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="U802" s="8"/>
       <c r="V802" s="48"/>
@@ -35506,7 +35488,7 @@
         <v>162</v>
       </c>
       <c r="N914" s="48" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="O914" s="7"/>
       <c r="P914" s="8"/>
@@ -44696,7 +44678,7 @@
         <v>157</v>
       </c>
       <c r="N1198" s="57" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="O1198" s="7"/>
       <c r="P1198" s="8"/>
@@ -47439,10 +47421,10 @@
       <c r="Q1283" s="8"/>
       <c r="R1283" s="8"/>
       <c r="S1283" s="8" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="T1283" s="8" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="U1283" s="8"/>
       <c r="V1283" s="48"/>
@@ -47681,7 +47663,7 @@
         <v>84</v>
       </c>
       <c r="T1290" s="8" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="U1290" s="8"/>
       <c r="V1290" s="48"/>
@@ -56730,7 +56712,7 @@
         <v>1167</v>
       </c>
       <c r="T1562" s="8" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="U1562" s="8"/>
       <c r="V1562" s="48" t="s">
@@ -57516,7 +57498,7 @@
         <v>1167</v>
       </c>
       <c r="T1588" s="1" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="V1588" s="48" t="s">
         <v>1155</v>
@@ -59524,7 +59506,7 @@
         <v>1167</v>
       </c>
       <c r="T1668" s="1" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="V1668" s="48"/>
     </row>
@@ -61185,7 +61167,7 @@
         <v>58</v>
       </c>
       <c r="N1729" s="48" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="O1729" s="8" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
nmv 22 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939255EC-423A-4439-8C8A-0753F15800A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046C51D-6970-4354-83D7-7A410AEC11D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T.S-7.3" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'T.S-7.3'!$C$1:$V$2124</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3429,9 +3429,6 @@
     <t>pari#gRuhItyai</t>
   </si>
   <si>
-    <t>saqdRu~g~g</t>
-  </si>
-  <si>
     <t>puqrohi#taH</t>
   </si>
   <si>
@@ -3543,9 +3540,6 @@
     <t>P[S]+N[S]</t>
   </si>
   <si>
-    <t>praqtya~g~g</t>
-  </si>
-  <si>
     <t>P[Sh]%S</t>
   </si>
   <si>
@@ -3574,13 +3568,19 @@
   </si>
   <si>
     <t>anvanu</t>
+  </si>
+  <si>
+    <t>praqtya~g</t>
+  </si>
+  <si>
+    <t>saqdRu~g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3730,8 +3730,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3753,6 +3759,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3784,7 +3796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3959,6 +3971,39 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4241,12 +4286,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2728"/>
+  <dimension ref="A1:V2124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2120" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2041" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2123" sqref="N2123"/>
+      <selection pane="bottomLeft" activeCell="O2125" sqref="O2125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -5050,10 +5095,10 @@
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
       <c r="S8" s="17" t="s">
+        <v>1165</v>
+      </c>
+      <c r="T8" s="17" t="s">
         <v>1166</v>
-      </c>
-      <c r="T8" s="17" t="s">
-        <v>1167</v>
       </c>
       <c r="U8" s="17"/>
       <c r="V8" s="47"/>
@@ -5330,10 +5375,10 @@
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="S15" s="17" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="T15" s="17" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="U15" s="17"/>
       <c r="V15" s="47"/>
@@ -6766,7 +6811,7 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N51" s="54" t="s">
+      <c r="N51" s="47" t="s">
         <v>111</v>
       </c>
       <c r="O51" s="7"/>
@@ -12217,7 +12262,7 @@
       <c r="T202" s="8"/>
       <c r="U202" s="8"/>
       <c r="V202" s="47" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="203" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -15337,7 +15382,7 @@
         <f t="shared" si="14"/>
         <v>91</v>
       </c>
-      <c r="N293" s="54" t="s">
+      <c r="N293" s="47" t="s">
         <v>214</v>
       </c>
       <c r="O293" s="7"/>
@@ -15350,39 +15395,39 @@
       <c r="T293" s="8"/>
       <c r="U293" s="8"/>
       <c r="V293" s="47" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="294" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A294" s="57"/>
       <c r="D294" s="24"/>
-      <c r="I294" s="50" t="s">
+      <c r="I294" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="J294" s="50">
+      <c r="J294" s="61">
         <v>7</v>
       </c>
-      <c r="K294" s="6">
+      <c r="K294" s="62">
         <f t="shared" si="12"/>
         <v>293</v>
       </c>
-      <c r="L294" s="6">
+      <c r="L294" s="62">
         <v>1</v>
       </c>
-      <c r="M294" s="6">
+      <c r="M294" s="62">
         <v>1</v>
       </c>
-      <c r="N294" s="47" t="s">
+      <c r="N294" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="O294" s="7"/>
-      <c r="P294" s="8"/>
-      <c r="Q294" s="8"/>
-      <c r="R294" s="8"/>
-      <c r="S294" s="8"/>
-      <c r="T294" s="8"/>
-      <c r="U294" s="8"/>
-      <c r="V294" s="47"/>
+      <c r="O294" s="12"/>
+      <c r="P294" s="13"/>
+      <c r="Q294" s="13"/>
+      <c r="R294" s="13"/>
+      <c r="S294" s="13"/>
+      <c r="T294" s="13"/>
+      <c r="U294" s="13"/>
+      <c r="V294" s="63"/>
     </row>
     <row r="295" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A295" s="57"/>
@@ -15693,10 +15738,10 @@
       <c r="Q303" s="8"/>
       <c r="R303" s="8"/>
       <c r="S303" s="17" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="T303" s="17" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="U303" s="8"/>
       <c r="V303" s="47"/>
@@ -17191,7 +17236,7 @@
         <f t="shared" si="17"/>
         <v>54</v>
       </c>
-      <c r="N347" s="47" t="s">
+      <c r="N347" s="60" t="s">
         <v>155</v>
       </c>
       <c r="O347" s="8" t="s">
@@ -17226,7 +17271,7 @@
         <f t="shared" si="17"/>
         <v>55</v>
       </c>
-      <c r="N348" s="47" t="s">
+      <c r="N348" s="60" t="s">
         <v>292</v>
       </c>
       <c r="O348" s="7"/>
@@ -17237,7 +17282,7 @@
         <v>206</v>
       </c>
       <c r="T348" s="8" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="U348" s="8"/>
       <c r="V348" s="47"/>
@@ -18571,7 +18616,7 @@
       <c r="T386" s="8"/>
       <c r="U386" s="8"/>
       <c r="V386" s="47" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="387" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -19303,7 +19348,7 @@
         <v>74</v>
       </c>
       <c r="T408" s="8" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="U408" s="8"/>
       <c r="V408" s="47"/>
@@ -19373,7 +19418,7 @@
         <v>74</v>
       </c>
       <c r="T410" s="8" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="U410" s="8"/>
       <c r="V410" s="47"/>
@@ -19744,7 +19789,7 @@
         <v>74</v>
       </c>
       <c r="T421" s="8" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="U421" s="8"/>
       <c r="V421" s="47"/>
@@ -19814,7 +19859,7 @@
         <v>74</v>
       </c>
       <c r="T423" s="8" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="U423" s="8"/>
       <c r="V423" s="47"/>
@@ -21398,7 +21443,7 @@
         <f t="shared" si="23"/>
         <v>84</v>
       </c>
-      <c r="N470" s="54" t="s">
+      <c r="N470" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="O470" s="8" t="s">
@@ -21413,7 +21458,7 @@
       <c r="T470" s="8"/>
       <c r="U470" s="8"/>
       <c r="V470" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="471" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -23510,7 +23555,7 @@
         <v>74</v>
       </c>
       <c r="T532" s="8" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="U532" s="8"/>
       <c r="V532" s="47"/>
@@ -23580,7 +23625,7 @@
         <v>74</v>
       </c>
       <c r="T534" s="8" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="U534" s="8"/>
       <c r="V534" s="47"/>
@@ -26315,8 +26360,8 @@
         <f t="shared" si="29"/>
         <v>145</v>
       </c>
-      <c r="N615" s="55" t="s">
-        <v>1171</v>
+      <c r="N615" s="64" t="s">
+        <v>1180</v>
       </c>
       <c r="O615" s="7"/>
       <c r="P615" s="8"/>
@@ -27578,7 +27623,7 @@
       <c r="T651" s="8"/>
       <c r="U651" s="8"/>
       <c r="V651" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="652" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -27667,8 +27712,8 @@
         <f t="shared" si="32"/>
         <v>3</v>
       </c>
-      <c r="N654" s="55" t="s">
-        <v>1133</v>
+      <c r="N654" s="64" t="s">
+        <v>1181</v>
       </c>
       <c r="O654" s="8" t="s">
         <v>62</v>
@@ -30836,7 +30881,7 @@
         <f t="shared" si="35"/>
         <v>101</v>
       </c>
-      <c r="N752" s="54" t="s">
+      <c r="N752" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="O752" s="8" t="s">
@@ -30851,7 +30896,7 @@
       <c r="T752" s="8"/>
       <c r="U752" s="8"/>
       <c r="V752" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="753" spans="8:22" x14ac:dyDescent="0.25">
@@ -31763,7 +31808,7 @@
         <v>84</v>
       </c>
       <c r="T780" s="8" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="U780" s="8"/>
       <c r="V780" s="47"/>
@@ -32480,7 +32525,7 @@
         <v>84</v>
       </c>
       <c r="T802" s="8" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="U802" s="8"/>
       <c r="V802" s="47"/>
@@ -33155,10 +33200,10 @@
       <c r="Q823" s="8"/>
       <c r="R823" s="8"/>
       <c r="S823" s="8" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="T823" s="8" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="U823" s="8"/>
       <c r="V823" s="47"/>
@@ -36082,8 +36127,8 @@
         <f t="shared" si="44"/>
         <v>162</v>
       </c>
-      <c r="N914" s="55" t="s">
-        <v>1171</v>
+      <c r="N914" s="64" t="s">
+        <v>1180</v>
       </c>
       <c r="O914" s="7"/>
       <c r="P914" s="8"/>
@@ -37394,7 +37439,7 @@
         <f t="shared" si="44"/>
         <v>202</v>
       </c>
-      <c r="N954" s="54" t="s">
+      <c r="N954" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="O954" s="8" t="s">
@@ -37409,7 +37454,7 @@
       <c r="T954" s="8"/>
       <c r="U954" s="8"/>
       <c r="V954" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="955" spans="9:22" x14ac:dyDescent="0.25">
@@ -40227,7 +40272,7 @@
         <f t="shared" si="50"/>
         <v>87</v>
       </c>
-      <c r="N1041" s="54" t="s">
+      <c r="N1041" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="O1041" s="8" t="s">
@@ -40242,7 +40287,7 @@
       <c r="T1041" s="8"/>
       <c r="U1041" s="8"/>
       <c r="V1041" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1042" spans="8:22" x14ac:dyDescent="0.25">
@@ -45266,8 +45311,8 @@
         <f t="shared" si="56"/>
         <v>157</v>
       </c>
-      <c r="N1198" s="55" t="s">
-        <v>1171</v>
+      <c r="N1198" s="64" t="s">
+        <v>1180</v>
       </c>
       <c r="O1198" s="7"/>
       <c r="P1198" s="8"/>
@@ -45792,7 +45837,7 @@
         <f t="shared" si="56"/>
         <v>173</v>
       </c>
-      <c r="N1214" s="54" t="s">
+      <c r="N1214" s="47" t="s">
         <v>1132</v>
       </c>
       <c r="O1214" s="8" t="s">
@@ -45807,7 +45852,7 @@
       <c r="T1214" s="8"/>
       <c r="U1214" s="8"/>
       <c r="V1214" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1215" spans="9:22" x14ac:dyDescent="0.25">
@@ -48010,10 +48055,10 @@
       <c r="Q1283" s="8"/>
       <c r="R1283" s="8"/>
       <c r="S1283" s="8" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="T1283" s="8" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="U1283" s="8"/>
       <c r="V1283" s="47"/>
@@ -48252,7 +48297,7 @@
         <v>84</v>
       </c>
       <c r="T1290" s="8" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="U1290" s="8"/>
       <c r="V1290" s="47"/>
@@ -49025,67 +49070,67 @@
     </row>
     <row r="1314" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1314" s="42"/>
-      <c r="I1314" s="50" t="s">
+      <c r="I1314" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="J1314" s="9">
+      <c r="J1314" s="66">
         <v>26</v>
       </c>
-      <c r="K1314" s="6">
+      <c r="K1314" s="67">
         <f t="shared" si="60"/>
         <v>1313</v>
       </c>
-      <c r="L1314" s="6">
+      <c r="L1314" s="67">
         <f t="shared" si="61"/>
         <v>50</v>
       </c>
-      <c r="M1314" s="6">
+      <c r="M1314" s="67">
         <f t="shared" si="62"/>
         <v>100</v>
       </c>
-      <c r="N1314" s="54" t="s">
+      <c r="N1314" s="68" t="s">
         <v>534</v>
       </c>
-      <c r="O1314" s="7"/>
-      <c r="P1314" s="8"/>
-      <c r="Q1314" s="8"/>
-      <c r="R1314" s="8"/>
-      <c r="S1314" s="8"/>
-      <c r="T1314" s="8"/>
-      <c r="U1314" s="8"/>
+      <c r="O1314" s="69"/>
+      <c r="P1314" s="70"/>
+      <c r="Q1314" s="70"/>
+      <c r="R1314" s="70"/>
+      <c r="S1314" s="70"/>
+      <c r="T1314" s="70"/>
+      <c r="U1314" s="70"/>
       <c r="V1314" s="47"/>
     </row>
     <row r="1315" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C1315" s="42"/>
-      <c r="I1315" s="50" t="s">
+      <c r="I1315" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="J1315" s="9">
+      <c r="J1315" s="66">
         <v>27</v>
       </c>
-      <c r="K1315" s="6">
+      <c r="K1315" s="67">
         <f t="shared" si="60"/>
         <v>1314</v>
       </c>
-      <c r="L1315" s="6">
+      <c r="L1315" s="67">
         <v>1</v>
       </c>
-      <c r="M1315" s="6">
+      <c r="M1315" s="67">
         <f t="shared" si="62"/>
         <v>101</v>
       </c>
-      <c r="N1315" s="47" t="s">
+      <c r="N1315" s="68" t="s">
         <v>280</v>
       </c>
-      <c r="O1315" s="8" t="s">
+      <c r="O1315" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="P1315" s="8"/>
-      <c r="Q1315" s="8"/>
-      <c r="R1315" s="8"/>
-      <c r="S1315" s="8"/>
-      <c r="T1315" s="8"/>
-      <c r="U1315" s="8"/>
+      <c r="P1315" s="70"/>
+      <c r="Q1315" s="70"/>
+      <c r="R1315" s="70"/>
+      <c r="S1315" s="70"/>
+      <c r="T1315" s="70"/>
+      <c r="U1315" s="70"/>
       <c r="V1315" s="47"/>
     </row>
     <row r="1316" spans="3:22" x14ac:dyDescent="0.25">
@@ -54735,7 +54780,7 @@
       <c r="T1485" s="8"/>
       <c r="U1485" s="8"/>
       <c r="V1485" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="1486" spans="3:22" x14ac:dyDescent="0.25">
@@ -54984,7 +55029,7 @@
         <f t="shared" si="71"/>
         <v>8</v>
       </c>
-      <c r="N1493" s="47" t="s">
+      <c r="N1493" s="68" t="s">
         <v>340</v>
       </c>
       <c r="O1493" s="7"/>
@@ -54997,7 +55042,7 @@
       <c r="T1493" s="8"/>
       <c r="U1493" s="8"/>
       <c r="V1493" s="47" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1494" spans="3:22" x14ac:dyDescent="0.25">
@@ -55085,7 +55130,7 @@
         <v>11</v>
       </c>
       <c r="N1496" s="47" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="O1496" s="8" t="s">
         <v>62</v>
@@ -55099,7 +55144,7 @@
       <c r="T1496" s="8"/>
       <c r="U1496" s="8"/>
       <c r="V1496" s="47" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="1497" spans="3:22" x14ac:dyDescent="0.25">
@@ -55396,7 +55441,7 @@
         <v>20</v>
       </c>
       <c r="N1505" s="47" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="O1505" s="7"/>
       <c r="P1505" s="8" t="s">
@@ -55408,7 +55453,7 @@
       <c r="T1505" s="8"/>
       <c r="U1505" s="8"/>
       <c r="V1505" s="47" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1506" spans="3:22" x14ac:dyDescent="0.25">
@@ -55665,7 +55710,7 @@
         <v>28</v>
       </c>
       <c r="N1513" s="47" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="O1513" s="7"/>
       <c r="P1513" s="8" t="s">
@@ -55677,7 +55722,7 @@
       <c r="T1513" s="8"/>
       <c r="U1513" s="8"/>
       <c r="V1513" s="47" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="1514" spans="3:22" x14ac:dyDescent="0.25">
@@ -55974,7 +56019,7 @@
       <c r="T1522" s="8"/>
       <c r="U1522" s="8"/>
       <c r="V1522" s="47" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="1523" spans="3:22" x14ac:dyDescent="0.25">
@@ -56298,7 +56343,7 @@
       <c r="T1532" s="8"/>
       <c r="U1532" s="8"/>
       <c r="V1532" s="47" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="1533" spans="3:22" x14ac:dyDescent="0.25">
@@ -56520,7 +56565,7 @@
       <c r="T1539" s="8"/>
       <c r="U1539" s="8"/>
       <c r="V1539" s="47" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1540" spans="9:22" x14ac:dyDescent="0.25">
@@ -56753,7 +56798,7 @@
       <c r="T1546" s="8"/>
       <c r="U1546" s="8"/>
       <c r="V1546" s="47" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="1547" spans="9:22" x14ac:dyDescent="0.25">
@@ -57062,7 +57107,7 @@
       <c r="T1555" s="8"/>
       <c r="U1555" s="8"/>
       <c r="V1555" s="47" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="1556" spans="5:22" x14ac:dyDescent="0.25">
@@ -57294,14 +57339,14 @@
       <c r="Q1562" s="8"/>
       <c r="R1562" s="8"/>
       <c r="S1562" s="8" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="T1562" s="8" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="U1562" s="8"/>
       <c r="V1562" s="47" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1563" spans="5:22" x14ac:dyDescent="0.25">
@@ -57492,7 +57537,7 @@
       <c r="T1568" s="8"/>
       <c r="U1568" s="8"/>
       <c r="V1568" s="47" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="1569" spans="9:22" x14ac:dyDescent="0.25">
@@ -57833,7 +57878,7 @@
         <v>94</v>
       </c>
       <c r="N1579" s="47" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="O1579" s="8" t="s">
         <v>62</v>
@@ -57847,7 +57892,7 @@
       <c r="T1579" s="8"/>
       <c r="U1579" s="8"/>
       <c r="V1579" s="47" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="1580" spans="9:22" x14ac:dyDescent="0.25">
@@ -58080,13 +58125,13 @@
         <v>63</v>
       </c>
       <c r="S1588" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="T1588" s="1" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="V1588" s="47" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="1589" spans="9:22" x14ac:dyDescent="0.25">
@@ -58341,7 +58386,7 @@
         <v>113</v>
       </c>
       <c r="N1598" s="47" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="P1598" s="8" t="s">
         <v>63</v>
@@ -58538,7 +58583,7 @@
         <v>63</v>
       </c>
       <c r="V1605" s="47" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="1606" spans="8:22" x14ac:dyDescent="0.25">
@@ -58843,13 +58888,13 @@
         <v>132</v>
       </c>
       <c r="N1617" s="47" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="P1617" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1617" s="47" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="1618" spans="9:22" x14ac:dyDescent="0.25">
@@ -60088,10 +60133,10 @@
         <v>672</v>
       </c>
       <c r="S1668" s="8" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="T1668" s="8" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="V1668" s="47"/>
     </row>
@@ -60169,7 +60214,7 @@
         <v>63</v>
       </c>
       <c r="V1671" s="47" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="1672" spans="8:22" x14ac:dyDescent="0.25">
@@ -60504,7 +60549,7 @@
         <v>12</v>
       </c>
       <c r="N1683" s="47" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="O1683" s="8" t="s">
         <v>62</v>
@@ -60513,7 +60558,7 @@
         <v>63</v>
       </c>
       <c r="V1683" s="47" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="1684" spans="8:22" x14ac:dyDescent="0.25">
@@ -60839,13 +60884,13 @@
         <v>24</v>
       </c>
       <c r="N1695" s="47" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P1695" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1695" s="47" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1696" spans="8:22" x14ac:dyDescent="0.25">
@@ -61127,7 +61172,7 @@
         <v>35</v>
       </c>
       <c r="N1706" s="47" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O1706" s="8" t="s">
         <v>64</v>
@@ -61136,7 +61181,7 @@
         <v>63</v>
       </c>
       <c r="V1706" s="47" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="1707" spans="9:22" x14ac:dyDescent="0.25">
@@ -61402,13 +61447,13 @@
         <v>46</v>
       </c>
       <c r="N1717" s="47" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P1717" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1717" s="47" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1718" spans="8:22" x14ac:dyDescent="0.25">
@@ -61720,7 +61765,7 @@
         <v>57</v>
       </c>
       <c r="N1728" s="47" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="O1728" s="8" t="s">
         <v>62</v>
@@ -61729,7 +61774,7 @@
         <v>63</v>
       </c>
       <c r="V1728" s="47" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1729" spans="1:22" x14ac:dyDescent="0.25">
@@ -61752,13 +61797,13 @@
         <v>58</v>
       </c>
       <c r="N1729" s="47" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="O1729" s="8" t="s">
         <v>62</v>
       </c>
       <c r="V1729" s="47" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1730" spans="1:22" x14ac:dyDescent="0.25">
@@ -62008,13 +62053,13 @@
         <v>68</v>
       </c>
       <c r="N1739" s="47" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P1739" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1739" s="47" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="1740" spans="1:22" x14ac:dyDescent="0.25">
@@ -62041,7 +62086,7 @@
     </row>
     <row r="1741" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1741" s="59" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="I1741" s="50" t="s">
         <v>54</v>
@@ -62068,7 +62113,7 @@
     </row>
     <row r="1742" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1742" s="59" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="I1742" s="50" t="s">
         <v>54</v>
@@ -63290,7 +63335,7 @@
         <v>63</v>
       </c>
       <c r="V1790" s="47" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="1791" spans="8:22" x14ac:dyDescent="0.25">
@@ -64783,14 +64828,14 @@
         <f t="shared" si="86"/>
         <v>60</v>
       </c>
-      <c r="N1850" s="54" t="s">
+      <c r="N1850" s="68" t="s">
         <v>653</v>
       </c>
       <c r="P1850" s="8" t="s">
         <v>63</v>
       </c>
       <c r="V1850" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1851" spans="9:22" x14ac:dyDescent="0.25">
@@ -67426,7 +67471,7 @@
         <v>63</v>
       </c>
       <c r="V1956" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1957" spans="9:22" x14ac:dyDescent="0.25">
@@ -68767,7 +68812,7 @@
         <v>63</v>
       </c>
       <c r="V2008" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="2009" spans="9:22" x14ac:dyDescent="0.25">
@@ -69904,7 +69949,7 @@
         <v>63</v>
       </c>
       <c r="V2054" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="2055" spans="9:22" x14ac:dyDescent="0.25">
@@ -70493,7 +70538,7 @@
         <v>63</v>
       </c>
       <c r="V2078" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="2079" spans="9:22" x14ac:dyDescent="0.25">
@@ -71650,3028 +71695,8 @@
         <v>63</v>
       </c>
       <c r="V2124" s="47" t="s">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="2125" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2125" s="50"/>
-      <c r="N2125" s="47"/>
-      <c r="V2125" s="47"/>
-    </row>
-    <row r="2126" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2126" s="50"/>
-      <c r="N2126" s="47"/>
-      <c r="V2126" s="47"/>
-    </row>
-    <row r="2127" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2127" s="50"/>
-      <c r="N2127" s="47"/>
-      <c r="V2127" s="47"/>
-    </row>
-    <row r="2128" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2128" s="50"/>
-      <c r="N2128" s="47"/>
-      <c r="V2128" s="47"/>
-    </row>
-    <row r="2129" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2129" s="50"/>
-      <c r="N2129" s="47"/>
-      <c r="V2129" s="47"/>
-    </row>
-    <row r="2130" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2130" s="50"/>
-      <c r="N2130" s="47"/>
-      <c r="V2130" s="47"/>
-    </row>
-    <row r="2131" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2131" s="50"/>
-      <c r="N2131" s="47"/>
-      <c r="V2131" s="47"/>
-    </row>
-    <row r="2132" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2132" s="50"/>
-      <c r="N2132" s="47"/>
-      <c r="V2132" s="47"/>
-    </row>
-    <row r="2133" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2133" s="50"/>
-      <c r="N2133" s="47"/>
-      <c r="V2133" s="47"/>
-    </row>
-    <row r="2134" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2134" s="50"/>
-      <c r="N2134" s="47"/>
-      <c r="V2134" s="47"/>
-    </row>
-    <row r="2135" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2135" s="50"/>
-      <c r="N2135" s="47"/>
-      <c r="V2135" s="47"/>
-    </row>
-    <row r="2136" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2136" s="50"/>
-      <c r="N2136" s="47"/>
-      <c r="V2136" s="47"/>
-    </row>
-    <row r="2137" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2137" s="50"/>
-      <c r="N2137" s="47"/>
-      <c r="V2137" s="47"/>
-    </row>
-    <row r="2138" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2138" s="50"/>
-      <c r="N2138" s="47"/>
-      <c r="V2138" s="47"/>
-    </row>
-    <row r="2139" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2139" s="50"/>
-      <c r="N2139" s="47"/>
-      <c r="V2139" s="47"/>
-    </row>
-    <row r="2140" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2140" s="50"/>
-      <c r="N2140" s="47"/>
-      <c r="V2140" s="47"/>
-    </row>
-    <row r="2141" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2141" s="50"/>
-      <c r="N2141" s="47"/>
-      <c r="V2141" s="47"/>
-    </row>
-    <row r="2142" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2142" s="50"/>
-      <c r="N2142" s="47"/>
-      <c r="V2142" s="47"/>
-    </row>
-    <row r="2143" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2143" s="50"/>
-      <c r="N2143" s="47"/>
-      <c r="V2143" s="47"/>
-    </row>
-    <row r="2144" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2144" s="50"/>
-      <c r="N2144" s="47"/>
-      <c r="V2144" s="47"/>
-    </row>
-    <row r="2145" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2145" s="50"/>
-      <c r="N2145" s="47"/>
-      <c r="V2145" s="47"/>
-    </row>
-    <row r="2146" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2146" s="50"/>
-      <c r="N2146" s="47"/>
-      <c r="V2146" s="47"/>
-    </row>
-    <row r="2147" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2147" s="50"/>
-      <c r="N2147" s="47"/>
-      <c r="V2147" s="47"/>
-    </row>
-    <row r="2148" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2148" s="50"/>
-      <c r="N2148" s="47"/>
-      <c r="V2148" s="47"/>
-    </row>
-    <row r="2149" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2149" s="50"/>
-      <c r="N2149" s="47"/>
-      <c r="V2149" s="47"/>
-    </row>
-    <row r="2150" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2150" s="50"/>
-      <c r="N2150" s="47"/>
-      <c r="V2150" s="47"/>
-    </row>
-    <row r="2151" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2151" s="50"/>
-      <c r="N2151" s="47"/>
-      <c r="V2151" s="47"/>
-    </row>
-    <row r="2152" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2152" s="50"/>
-      <c r="N2152" s="47"/>
-      <c r="V2152" s="47"/>
-    </row>
-    <row r="2153" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2153" s="50"/>
-      <c r="N2153" s="47"/>
-      <c r="V2153" s="47"/>
-    </row>
-    <row r="2154" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2154" s="50"/>
-      <c r="N2154" s="47"/>
-      <c r="V2154" s="47"/>
-    </row>
-    <row r="2155" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2155" s="50"/>
-      <c r="N2155" s="47"/>
-      <c r="V2155" s="47"/>
-    </row>
-    <row r="2156" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2156" s="50"/>
-      <c r="N2156" s="47"/>
-      <c r="V2156" s="47"/>
-    </row>
-    <row r="2157" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2157" s="50"/>
-      <c r="N2157" s="47"/>
-      <c r="V2157" s="47"/>
-    </row>
-    <row r="2158" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2158" s="50"/>
-      <c r="N2158" s="47"/>
-      <c r="V2158" s="47"/>
-    </row>
-    <row r="2159" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2159" s="50"/>
-      <c r="N2159" s="47"/>
-      <c r="V2159" s="47"/>
-    </row>
-    <row r="2160" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2160" s="50"/>
-      <c r="N2160" s="47"/>
-      <c r="V2160" s="47"/>
-    </row>
-    <row r="2161" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2161" s="50"/>
-      <c r="N2161" s="47"/>
-      <c r="V2161" s="47"/>
-    </row>
-    <row r="2162" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2162" s="50"/>
-      <c r="N2162" s="47"/>
-      <c r="V2162" s="47"/>
-    </row>
-    <row r="2163" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2163" s="50"/>
-      <c r="N2163" s="47"/>
-      <c r="V2163" s="47"/>
-    </row>
-    <row r="2164" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2164" s="50"/>
-      <c r="N2164" s="47"/>
-      <c r="V2164" s="47"/>
-    </row>
-    <row r="2165" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2165" s="50"/>
-      <c r="N2165" s="47"/>
-      <c r="V2165" s="47"/>
-    </row>
-    <row r="2166" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2166" s="50"/>
-      <c r="N2166" s="47"/>
-      <c r="V2166" s="47"/>
-    </row>
-    <row r="2167" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2167" s="50"/>
-      <c r="N2167" s="47"/>
-      <c r="V2167" s="47"/>
-    </row>
-    <row r="2168" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2168" s="50"/>
-      <c r="N2168" s="47"/>
-      <c r="V2168" s="47"/>
-    </row>
-    <row r="2169" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2169" s="50"/>
-      <c r="N2169" s="47"/>
-      <c r="V2169" s="47"/>
-    </row>
-    <row r="2170" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2170" s="50"/>
-      <c r="N2170" s="47"/>
-      <c r="V2170" s="47"/>
-    </row>
-    <row r="2171" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2171" s="50"/>
-      <c r="N2171" s="47"/>
-      <c r="V2171" s="47"/>
-    </row>
-    <row r="2172" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2172" s="50"/>
-      <c r="N2172" s="47"/>
-      <c r="V2172" s="47"/>
-    </row>
-    <row r="2173" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2173" s="50"/>
-      <c r="N2173" s="47"/>
-      <c r="V2173" s="47"/>
-    </row>
-    <row r="2174" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2174" s="50"/>
-      <c r="N2174" s="47"/>
-      <c r="V2174" s="47"/>
-    </row>
-    <row r="2175" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2175" s="50"/>
-      <c r="N2175" s="47"/>
-      <c r="V2175" s="47"/>
-    </row>
-    <row r="2176" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2176" s="50"/>
-      <c r="N2176" s="47"/>
-      <c r="V2176" s="47"/>
-    </row>
-    <row r="2177" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2177" s="50"/>
-      <c r="N2177" s="47"/>
-      <c r="V2177" s="47"/>
-    </row>
-    <row r="2178" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2178" s="50"/>
-      <c r="N2178" s="47"/>
-      <c r="V2178" s="47"/>
-    </row>
-    <row r="2179" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2179" s="50"/>
-      <c r="N2179" s="47"/>
-      <c r="V2179" s="47"/>
-    </row>
-    <row r="2180" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2180" s="50"/>
-      <c r="N2180" s="47"/>
-      <c r="V2180" s="47"/>
-    </row>
-    <row r="2181" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2181" s="50"/>
-      <c r="N2181" s="47"/>
-      <c r="V2181" s="47"/>
-    </row>
-    <row r="2182" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2182" s="50"/>
-      <c r="N2182" s="47"/>
-      <c r="V2182" s="47"/>
-    </row>
-    <row r="2183" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2183" s="50"/>
-      <c r="N2183" s="47"/>
-      <c r="V2183" s="47"/>
-    </row>
-    <row r="2184" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2184" s="50"/>
-      <c r="N2184" s="47"/>
-      <c r="V2184" s="47"/>
-    </row>
-    <row r="2185" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2185" s="50"/>
-      <c r="N2185" s="47"/>
-      <c r="V2185" s="47"/>
-    </row>
-    <row r="2186" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2186" s="50"/>
-      <c r="N2186" s="47"/>
-      <c r="V2186" s="47"/>
-    </row>
-    <row r="2187" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2187" s="50"/>
-      <c r="N2187" s="47"/>
-      <c r="V2187" s="47"/>
-    </row>
-    <row r="2188" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2188" s="50"/>
-      <c r="N2188" s="47"/>
-      <c r="V2188" s="47"/>
-    </row>
-    <row r="2189" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2189" s="50"/>
-      <c r="N2189" s="47"/>
-      <c r="V2189" s="47"/>
-    </row>
-    <row r="2190" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2190" s="50"/>
-      <c r="N2190" s="47"/>
-      <c r="V2190" s="47"/>
-    </row>
-    <row r="2191" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2191" s="50"/>
-      <c r="N2191" s="47"/>
-      <c r="V2191" s="47"/>
-    </row>
-    <row r="2192" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2192" s="50"/>
-      <c r="N2192" s="47"/>
-      <c r="V2192" s="47"/>
-    </row>
-    <row r="2193" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2193" s="50"/>
-      <c r="N2193" s="47"/>
-      <c r="V2193" s="47"/>
-    </row>
-    <row r="2194" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2194" s="50"/>
-      <c r="N2194" s="47"/>
-      <c r="V2194" s="47"/>
-    </row>
-    <row r="2195" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2195" s="50"/>
-      <c r="N2195" s="47"/>
-      <c r="V2195" s="47"/>
-    </row>
-    <row r="2196" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2196" s="50"/>
-      <c r="N2196" s="47"/>
-      <c r="V2196" s="47"/>
-    </row>
-    <row r="2197" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2197" s="50"/>
-      <c r="N2197" s="47"/>
-      <c r="V2197" s="47"/>
-    </row>
-    <row r="2198" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2198" s="50"/>
-      <c r="N2198" s="47"/>
-      <c r="V2198" s="47"/>
-    </row>
-    <row r="2199" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2199" s="50"/>
-      <c r="N2199" s="47"/>
-      <c r="V2199" s="47"/>
-    </row>
-    <row r="2200" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2200" s="50"/>
-      <c r="N2200" s="47"/>
-      <c r="V2200" s="47"/>
-    </row>
-    <row r="2201" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2201" s="50"/>
-      <c r="N2201" s="47"/>
-      <c r="V2201" s="47"/>
-    </row>
-    <row r="2202" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2202" s="50"/>
-      <c r="N2202" s="47"/>
-      <c r="V2202" s="47"/>
-    </row>
-    <row r="2203" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2203" s="50"/>
-      <c r="N2203" s="47"/>
-      <c r="V2203" s="47"/>
-    </row>
-    <row r="2204" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2204" s="50"/>
-      <c r="N2204" s="47"/>
-      <c r="V2204" s="47"/>
-    </row>
-    <row r="2205" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2205" s="50"/>
-      <c r="N2205" s="47"/>
-      <c r="V2205" s="47"/>
-    </row>
-    <row r="2206" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2206" s="50"/>
-      <c r="N2206" s="47"/>
-      <c r="V2206" s="47"/>
-    </row>
-    <row r="2207" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2207" s="50"/>
-      <c r="N2207" s="47"/>
-      <c r="V2207" s="47"/>
-    </row>
-    <row r="2208" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2208" s="50"/>
-      <c r="N2208" s="47"/>
-      <c r="V2208" s="47"/>
-    </row>
-    <row r="2209" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2209" s="50"/>
-      <c r="N2209" s="47"/>
-      <c r="V2209" s="47"/>
-    </row>
-    <row r="2210" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2210" s="50"/>
-      <c r="N2210" s="47"/>
-      <c r="V2210" s="47"/>
-    </row>
-    <row r="2211" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2211" s="50"/>
-      <c r="N2211" s="47"/>
-      <c r="V2211" s="47"/>
-    </row>
-    <row r="2212" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2212" s="50"/>
-      <c r="N2212" s="47"/>
-      <c r="V2212" s="47"/>
-    </row>
-    <row r="2213" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2213" s="50"/>
-      <c r="N2213" s="47"/>
-      <c r="V2213" s="47"/>
-    </row>
-    <row r="2214" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2214" s="50"/>
-      <c r="N2214" s="47"/>
-      <c r="V2214" s="47"/>
-    </row>
-    <row r="2215" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2215" s="50"/>
-      <c r="N2215" s="47"/>
-      <c r="V2215" s="47"/>
-    </row>
-    <row r="2216" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2216" s="50"/>
-      <c r="N2216" s="47"/>
-      <c r="V2216" s="47"/>
-    </row>
-    <row r="2217" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2217" s="50"/>
-      <c r="N2217" s="47"/>
-      <c r="V2217" s="47"/>
-    </row>
-    <row r="2218" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2218" s="50"/>
-      <c r="N2218" s="47"/>
-      <c r="V2218" s="47"/>
-    </row>
-    <row r="2219" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2219" s="50"/>
-      <c r="N2219" s="47"/>
-      <c r="V2219" s="47"/>
-    </row>
-    <row r="2220" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2220" s="50"/>
-      <c r="N2220" s="47"/>
-      <c r="V2220" s="47"/>
-    </row>
-    <row r="2221" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2221" s="50"/>
-      <c r="N2221" s="47"/>
-      <c r="V2221" s="47"/>
-    </row>
-    <row r="2222" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2222" s="50"/>
-      <c r="N2222" s="47"/>
-      <c r="V2222" s="47"/>
-    </row>
-    <row r="2223" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2223" s="50"/>
-      <c r="N2223" s="47"/>
-      <c r="V2223" s="47"/>
-    </row>
-    <row r="2224" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2224" s="50"/>
-      <c r="N2224" s="47"/>
-      <c r="V2224" s="47"/>
-    </row>
-    <row r="2225" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2225" s="50"/>
-      <c r="N2225" s="47"/>
-      <c r="V2225" s="47"/>
-    </row>
-    <row r="2226" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2226" s="50"/>
-      <c r="N2226" s="47"/>
-      <c r="V2226" s="47"/>
-    </row>
-    <row r="2227" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2227" s="50"/>
-      <c r="N2227" s="47"/>
-      <c r="V2227" s="47"/>
-    </row>
-    <row r="2228" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2228" s="50"/>
-      <c r="N2228" s="47"/>
-      <c r="V2228" s="47"/>
-    </row>
-    <row r="2229" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2229" s="50"/>
-      <c r="N2229" s="47"/>
-      <c r="V2229" s="47"/>
-    </row>
-    <row r="2230" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2230" s="50"/>
-      <c r="N2230" s="47"/>
-      <c r="V2230" s="47"/>
-    </row>
-    <row r="2231" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2231" s="50"/>
-      <c r="N2231" s="47"/>
-      <c r="V2231" s="47"/>
-    </row>
-    <row r="2232" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2232" s="50"/>
-      <c r="N2232" s="47"/>
-      <c r="V2232" s="47"/>
-    </row>
-    <row r="2233" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2233" s="50"/>
-      <c r="N2233" s="47"/>
-      <c r="V2233" s="47"/>
-    </row>
-    <row r="2234" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2234" s="50"/>
-      <c r="N2234" s="47"/>
-      <c r="V2234" s="47"/>
-    </row>
-    <row r="2235" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2235" s="50"/>
-      <c r="N2235" s="47"/>
-      <c r="V2235" s="47"/>
-    </row>
-    <row r="2236" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2236" s="50"/>
-      <c r="N2236" s="47"/>
-      <c r="V2236" s="47"/>
-    </row>
-    <row r="2237" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2237" s="50"/>
-      <c r="N2237" s="47"/>
-      <c r="V2237" s="47"/>
-    </row>
-    <row r="2238" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2238" s="50"/>
-      <c r="N2238" s="47"/>
-      <c r="V2238" s="47"/>
-    </row>
-    <row r="2239" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2239" s="50"/>
-      <c r="N2239" s="47"/>
-      <c r="V2239" s="47"/>
-    </row>
-    <row r="2240" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2240" s="50"/>
-      <c r="N2240" s="47"/>
-      <c r="V2240" s="47"/>
-    </row>
-    <row r="2241" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2241" s="50"/>
-      <c r="N2241" s="47"/>
-      <c r="V2241" s="47"/>
-    </row>
-    <row r="2242" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2242" s="50"/>
-      <c r="N2242" s="47"/>
-      <c r="V2242" s="47"/>
-    </row>
-    <row r="2243" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2243" s="50"/>
-      <c r="N2243" s="47"/>
-      <c r="V2243" s="47"/>
-    </row>
-    <row r="2244" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2244" s="50"/>
-      <c r="N2244" s="47"/>
-      <c r="V2244" s="47"/>
-    </row>
-    <row r="2245" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2245" s="50"/>
-      <c r="N2245" s="47"/>
-      <c r="V2245" s="47"/>
-    </row>
-    <row r="2246" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2246" s="50"/>
-      <c r="N2246" s="47"/>
-      <c r="V2246" s="47"/>
-    </row>
-    <row r="2247" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2247" s="50"/>
-      <c r="N2247" s="47"/>
-      <c r="V2247" s="47"/>
-    </row>
-    <row r="2248" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2248" s="50"/>
-      <c r="N2248" s="47"/>
-      <c r="V2248" s="47"/>
-    </row>
-    <row r="2249" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2249" s="50"/>
-      <c r="N2249" s="47"/>
-      <c r="V2249" s="47"/>
-    </row>
-    <row r="2250" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2250" s="50"/>
-      <c r="N2250" s="47"/>
-      <c r="V2250" s="47"/>
-    </row>
-    <row r="2251" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2251" s="50"/>
-      <c r="N2251" s="47"/>
-      <c r="V2251" s="47"/>
-    </row>
-    <row r="2252" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2252" s="50"/>
-      <c r="N2252" s="47"/>
-      <c r="V2252" s="47"/>
-    </row>
-    <row r="2253" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2253" s="50"/>
-      <c r="N2253" s="47"/>
-      <c r="V2253" s="47"/>
-    </row>
-    <row r="2254" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2254" s="50"/>
-      <c r="N2254" s="47"/>
-      <c r="V2254" s="47"/>
-    </row>
-    <row r="2255" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2255" s="50"/>
-      <c r="N2255" s="47"/>
-      <c r="V2255" s="47"/>
-    </row>
-    <row r="2256" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2256" s="50"/>
-      <c r="N2256" s="47"/>
-      <c r="V2256" s="47"/>
-    </row>
-    <row r="2257" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2257" s="50"/>
-      <c r="N2257" s="47"/>
-      <c r="V2257" s="47"/>
-    </row>
-    <row r="2258" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2258" s="50"/>
-      <c r="N2258" s="47"/>
-      <c r="V2258" s="47"/>
-    </row>
-    <row r="2259" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2259" s="50"/>
-      <c r="N2259" s="47"/>
-      <c r="V2259" s="47"/>
-    </row>
-    <row r="2260" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2260" s="50"/>
-      <c r="N2260" s="47"/>
-      <c r="V2260" s="47"/>
-    </row>
-    <row r="2261" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2261" s="50"/>
-      <c r="N2261" s="47"/>
-      <c r="V2261" s="47"/>
-    </row>
-    <row r="2262" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2262" s="50"/>
-      <c r="N2262" s="47"/>
-      <c r="V2262" s="47"/>
-    </row>
-    <row r="2263" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2263" s="50"/>
-      <c r="N2263" s="47"/>
-      <c r="V2263" s="47"/>
-    </row>
-    <row r="2264" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2264" s="50"/>
-      <c r="N2264" s="47"/>
-      <c r="V2264" s="47"/>
-    </row>
-    <row r="2265" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2265" s="50"/>
-      <c r="N2265" s="47"/>
-      <c r="V2265" s="47"/>
-    </row>
-    <row r="2266" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2266" s="50"/>
-      <c r="N2266" s="47"/>
-      <c r="V2266" s="47"/>
-    </row>
-    <row r="2267" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2267" s="50"/>
-      <c r="N2267" s="47"/>
-      <c r="V2267" s="47"/>
-    </row>
-    <row r="2268" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2268" s="50"/>
-      <c r="N2268" s="47"/>
-      <c r="V2268" s="47"/>
-    </row>
-    <row r="2269" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2269" s="50"/>
-      <c r="N2269" s="47"/>
-      <c r="V2269" s="47"/>
-    </row>
-    <row r="2270" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2270" s="50"/>
-      <c r="N2270" s="47"/>
-      <c r="V2270" s="47"/>
-    </row>
-    <row r="2271" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2271" s="50"/>
-      <c r="N2271" s="47"/>
-      <c r="V2271" s="47"/>
-    </row>
-    <row r="2272" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2272" s="50"/>
-      <c r="N2272" s="47"/>
-      <c r="V2272" s="47"/>
-    </row>
-    <row r="2273" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2273" s="50"/>
-      <c r="N2273" s="47"/>
-      <c r="V2273" s="47"/>
-    </row>
-    <row r="2274" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2274" s="50"/>
-      <c r="N2274" s="47"/>
-      <c r="V2274" s="47"/>
-    </row>
-    <row r="2275" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2275" s="50"/>
-      <c r="N2275" s="47"/>
-      <c r="V2275" s="47"/>
-    </row>
-    <row r="2276" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2276" s="50"/>
-      <c r="N2276" s="47"/>
-      <c r="V2276" s="47"/>
-    </row>
-    <row r="2277" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2277" s="50"/>
-      <c r="N2277" s="47"/>
-      <c r="V2277" s="47"/>
-    </row>
-    <row r="2278" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2278" s="50"/>
-      <c r="N2278" s="47"/>
-      <c r="V2278" s="47"/>
-    </row>
-    <row r="2279" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2279" s="50"/>
-      <c r="N2279" s="47"/>
-      <c r="V2279" s="47"/>
-    </row>
-    <row r="2280" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2280" s="50"/>
-      <c r="N2280" s="47"/>
-      <c r="V2280" s="47"/>
-    </row>
-    <row r="2281" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2281" s="50"/>
-      <c r="N2281" s="47"/>
-      <c r="V2281" s="47"/>
-    </row>
-    <row r="2282" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2282" s="50"/>
-      <c r="N2282" s="47"/>
-      <c r="V2282" s="47"/>
-    </row>
-    <row r="2283" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2283" s="50"/>
-      <c r="N2283" s="47"/>
-      <c r="V2283" s="47"/>
-    </row>
-    <row r="2284" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2284" s="50"/>
-      <c r="N2284" s="47"/>
-      <c r="V2284" s="47"/>
-    </row>
-    <row r="2285" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2285" s="50"/>
-      <c r="N2285" s="47"/>
-      <c r="V2285" s="47"/>
-    </row>
-    <row r="2286" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2286" s="50"/>
-      <c r="N2286" s="47"/>
-      <c r="V2286" s="47"/>
-    </row>
-    <row r="2287" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2287" s="50"/>
-      <c r="N2287" s="47"/>
-      <c r="V2287" s="47"/>
-    </row>
-    <row r="2288" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2288" s="50"/>
-      <c r="N2288" s="47"/>
-      <c r="V2288" s="47"/>
-    </row>
-    <row r="2289" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2289" s="50"/>
-      <c r="N2289" s="47"/>
-      <c r="V2289" s="47"/>
-    </row>
-    <row r="2290" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2290" s="50"/>
-      <c r="N2290" s="47"/>
-      <c r="V2290" s="47"/>
-    </row>
-    <row r="2291" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2291" s="50"/>
-      <c r="N2291" s="47"/>
-      <c r="V2291" s="47"/>
-    </row>
-    <row r="2292" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2292" s="50"/>
-      <c r="N2292" s="47"/>
-      <c r="V2292" s="47"/>
-    </row>
-    <row r="2293" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2293" s="50"/>
-      <c r="N2293" s="47"/>
-      <c r="V2293" s="47"/>
-    </row>
-    <row r="2294" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2294" s="50"/>
-      <c r="N2294" s="47"/>
-      <c r="V2294" s="47"/>
-    </row>
-    <row r="2295" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2295" s="50"/>
-      <c r="N2295" s="47"/>
-      <c r="V2295" s="47"/>
-    </row>
-    <row r="2296" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2296" s="50"/>
-      <c r="N2296" s="47"/>
-      <c r="V2296" s="47"/>
-    </row>
-    <row r="2297" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2297" s="50"/>
-      <c r="N2297" s="47"/>
-      <c r="V2297" s="47"/>
-    </row>
-    <row r="2298" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2298" s="50"/>
-      <c r="N2298" s="47"/>
-      <c r="V2298" s="47"/>
-    </row>
-    <row r="2299" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2299" s="50"/>
-      <c r="N2299" s="47"/>
-      <c r="V2299" s="47"/>
-    </row>
-    <row r="2300" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2300" s="50"/>
-      <c r="N2300" s="47"/>
-      <c r="V2300" s="47"/>
-    </row>
-    <row r="2301" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2301" s="50"/>
-      <c r="N2301" s="47"/>
-      <c r="V2301" s="47"/>
-    </row>
-    <row r="2302" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2302" s="50"/>
-      <c r="N2302" s="47"/>
-      <c r="V2302" s="47"/>
-    </row>
-    <row r="2303" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2303" s="50"/>
-      <c r="N2303" s="47"/>
-      <c r="V2303" s="47"/>
-    </row>
-    <row r="2304" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2304" s="50"/>
-      <c r="N2304" s="47"/>
-      <c r="V2304" s="47"/>
-    </row>
-    <row r="2305" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2305" s="50"/>
-      <c r="N2305" s="47"/>
-      <c r="V2305" s="47"/>
-    </row>
-    <row r="2306" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2306" s="50"/>
-      <c r="N2306" s="47"/>
-      <c r="V2306" s="47"/>
-    </row>
-    <row r="2307" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2307" s="50"/>
-      <c r="N2307" s="47"/>
-      <c r="V2307" s="47"/>
-    </row>
-    <row r="2308" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2308" s="50"/>
-      <c r="N2308" s="47"/>
-      <c r="V2308" s="47"/>
-    </row>
-    <row r="2309" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2309" s="50"/>
-      <c r="N2309" s="47"/>
-      <c r="V2309" s="47"/>
-    </row>
-    <row r="2310" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2310" s="50"/>
-      <c r="N2310" s="47"/>
-      <c r="V2310" s="47"/>
-    </row>
-    <row r="2311" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2311" s="50"/>
-      <c r="N2311" s="47"/>
-      <c r="V2311" s="47"/>
-    </row>
-    <row r="2312" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2312" s="50"/>
-      <c r="N2312" s="47"/>
-      <c r="V2312" s="47"/>
-    </row>
-    <row r="2313" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2313" s="50"/>
-      <c r="N2313" s="47"/>
-      <c r="V2313" s="47"/>
-    </row>
-    <row r="2314" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2314" s="50"/>
-      <c r="N2314" s="47"/>
-      <c r="V2314" s="47"/>
-    </row>
-    <row r="2315" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2315" s="50"/>
-      <c r="N2315" s="47"/>
-      <c r="V2315" s="47"/>
-    </row>
-    <row r="2316" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2316" s="50"/>
-      <c r="N2316" s="47"/>
-      <c r="V2316" s="47"/>
-    </row>
-    <row r="2317" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2317" s="50"/>
-      <c r="N2317" s="47"/>
-      <c r="V2317" s="47"/>
-    </row>
-    <row r="2318" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2318" s="50"/>
-      <c r="N2318" s="47"/>
-      <c r="V2318" s="47"/>
-    </row>
-    <row r="2319" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2319" s="50"/>
-      <c r="N2319" s="47"/>
-      <c r="V2319" s="47"/>
-    </row>
-    <row r="2320" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2320" s="50"/>
-      <c r="N2320" s="47"/>
-      <c r="V2320" s="47"/>
-    </row>
-    <row r="2321" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2321" s="50"/>
-      <c r="N2321" s="47"/>
-      <c r="V2321" s="47"/>
-    </row>
-    <row r="2322" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2322" s="50"/>
-      <c r="N2322" s="47"/>
-      <c r="V2322" s="47"/>
-    </row>
-    <row r="2323" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2323" s="50"/>
-      <c r="N2323" s="47"/>
-      <c r="V2323" s="47"/>
-    </row>
-    <row r="2324" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2324" s="50"/>
-      <c r="N2324" s="47"/>
-      <c r="V2324" s="47"/>
-    </row>
-    <row r="2325" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2325" s="50"/>
-      <c r="N2325" s="47"/>
-      <c r="V2325" s="47"/>
-    </row>
-    <row r="2326" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2326" s="50"/>
-      <c r="N2326" s="47"/>
-      <c r="V2326" s="47"/>
-    </row>
-    <row r="2327" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2327" s="50"/>
-      <c r="N2327" s="47"/>
-      <c r="V2327" s="47"/>
-    </row>
-    <row r="2328" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2328" s="50"/>
-      <c r="N2328" s="47"/>
-      <c r="V2328" s="47"/>
-    </row>
-    <row r="2329" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2329" s="50"/>
-      <c r="N2329" s="47"/>
-      <c r="V2329" s="47"/>
-    </row>
-    <row r="2330" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2330" s="50"/>
-      <c r="N2330" s="47"/>
-      <c r="V2330" s="47"/>
-    </row>
-    <row r="2331" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2331" s="50"/>
-      <c r="N2331" s="47"/>
-      <c r="V2331" s="47"/>
-    </row>
-    <row r="2332" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2332" s="50"/>
-      <c r="N2332" s="47"/>
-      <c r="V2332" s="47"/>
-    </row>
-    <row r="2333" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2333" s="50"/>
-      <c r="N2333" s="47"/>
-      <c r="V2333" s="47"/>
-    </row>
-    <row r="2334" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2334" s="50"/>
-      <c r="N2334" s="47"/>
-      <c r="V2334" s="47"/>
-    </row>
-    <row r="2335" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2335" s="50"/>
-      <c r="N2335" s="47"/>
-      <c r="V2335" s="47"/>
-    </row>
-    <row r="2336" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2336" s="50"/>
-      <c r="N2336" s="47"/>
-      <c r="V2336" s="47"/>
-    </row>
-    <row r="2337" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2337" s="50"/>
-      <c r="N2337" s="47"/>
-      <c r="V2337" s="47"/>
-    </row>
-    <row r="2338" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2338" s="50"/>
-      <c r="N2338" s="47"/>
-      <c r="V2338" s="47"/>
-    </row>
-    <row r="2339" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2339" s="50"/>
-      <c r="N2339" s="47"/>
-      <c r="V2339" s="47"/>
-    </row>
-    <row r="2340" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2340" s="50"/>
-      <c r="N2340" s="47"/>
-      <c r="V2340" s="47"/>
-    </row>
-    <row r="2341" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2341" s="50"/>
-      <c r="N2341" s="47"/>
-      <c r="V2341" s="47"/>
-    </row>
-    <row r="2342" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2342" s="50"/>
-      <c r="N2342" s="47"/>
-      <c r="V2342" s="47"/>
-    </row>
-    <row r="2343" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2343" s="50"/>
-      <c r="N2343" s="47"/>
-      <c r="V2343" s="47"/>
-    </row>
-    <row r="2344" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2344" s="50"/>
-      <c r="N2344" s="47"/>
-      <c r="V2344" s="47"/>
-    </row>
-    <row r="2345" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2345" s="50"/>
-      <c r="N2345" s="47"/>
-      <c r="V2345" s="47"/>
-    </row>
-    <row r="2346" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2346" s="50"/>
-      <c r="N2346" s="47"/>
-      <c r="V2346" s="47"/>
-    </row>
-    <row r="2347" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2347" s="50"/>
-      <c r="N2347" s="47"/>
-      <c r="V2347" s="47"/>
-    </row>
-    <row r="2348" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2348" s="50"/>
-      <c r="N2348" s="47"/>
-      <c r="V2348" s="47"/>
-    </row>
-    <row r="2349" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2349" s="50"/>
-      <c r="N2349" s="47"/>
-      <c r="V2349" s="47"/>
-    </row>
-    <row r="2350" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2350" s="50"/>
-      <c r="N2350" s="47"/>
-      <c r="V2350" s="47"/>
-    </row>
-    <row r="2351" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2351" s="50"/>
-      <c r="N2351" s="47"/>
-      <c r="V2351" s="47"/>
-    </row>
-    <row r="2352" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2352" s="50"/>
-      <c r="N2352" s="47"/>
-      <c r="V2352" s="47"/>
-    </row>
-    <row r="2353" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2353" s="50"/>
-      <c r="N2353" s="47"/>
-      <c r="V2353" s="47"/>
-    </row>
-    <row r="2354" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2354" s="50"/>
-      <c r="N2354" s="47"/>
-      <c r="V2354" s="47"/>
-    </row>
-    <row r="2355" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2355" s="50"/>
-      <c r="N2355" s="47"/>
-      <c r="V2355" s="47"/>
-    </row>
-    <row r="2356" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2356" s="50"/>
-      <c r="N2356" s="47"/>
-      <c r="V2356" s="47"/>
-    </row>
-    <row r="2357" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2357" s="50"/>
-      <c r="N2357" s="47"/>
-      <c r="V2357" s="47"/>
-    </row>
-    <row r="2358" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2358" s="50"/>
-      <c r="N2358" s="47"/>
-      <c r="V2358" s="47"/>
-    </row>
-    <row r="2359" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2359" s="50"/>
-      <c r="N2359" s="47"/>
-      <c r="V2359" s="47"/>
-    </row>
-    <row r="2360" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2360" s="50"/>
-      <c r="N2360" s="47"/>
-      <c r="V2360" s="47"/>
-    </row>
-    <row r="2361" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2361" s="50"/>
-      <c r="N2361" s="47"/>
-      <c r="V2361" s="47"/>
-    </row>
-    <row r="2362" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2362" s="50"/>
-      <c r="N2362" s="47"/>
-      <c r="V2362" s="47"/>
-    </row>
-    <row r="2363" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2363" s="50"/>
-      <c r="N2363" s="47"/>
-      <c r="V2363" s="47"/>
-    </row>
-    <row r="2364" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2364" s="50"/>
-      <c r="N2364" s="47"/>
-      <c r="V2364" s="47"/>
-    </row>
-    <row r="2365" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2365" s="50"/>
-      <c r="N2365" s="47"/>
-      <c r="V2365" s="47"/>
-    </row>
-    <row r="2366" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2366" s="50"/>
-      <c r="N2366" s="47"/>
-      <c r="V2366" s="47"/>
-    </row>
-    <row r="2367" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2367" s="50"/>
-      <c r="N2367" s="47"/>
-      <c r="V2367" s="47"/>
-    </row>
-    <row r="2368" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2368" s="50"/>
-      <c r="N2368" s="47"/>
-      <c r="V2368" s="47"/>
-    </row>
-    <row r="2369" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2369" s="50"/>
-      <c r="N2369" s="47"/>
-      <c r="V2369" s="47"/>
-    </row>
-    <row r="2370" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2370" s="50"/>
-      <c r="N2370" s="47"/>
-      <c r="V2370" s="47"/>
-    </row>
-    <row r="2371" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2371" s="50"/>
-      <c r="N2371" s="47"/>
-      <c r="V2371" s="47"/>
-    </row>
-    <row r="2372" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2372" s="50"/>
-      <c r="N2372" s="47"/>
-      <c r="V2372" s="47"/>
-    </row>
-    <row r="2373" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2373" s="50"/>
-      <c r="N2373" s="47"/>
-      <c r="V2373" s="47"/>
-    </row>
-    <row r="2374" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2374" s="50"/>
-      <c r="N2374" s="47"/>
-      <c r="V2374" s="47"/>
-    </row>
-    <row r="2375" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2375" s="50"/>
-      <c r="N2375" s="47"/>
-      <c r="V2375" s="47"/>
-    </row>
-    <row r="2376" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2376" s="50"/>
-      <c r="N2376" s="47"/>
-      <c r="V2376" s="47"/>
-    </row>
-    <row r="2377" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2377" s="50"/>
-      <c r="N2377" s="47"/>
-      <c r="V2377" s="47"/>
-    </row>
-    <row r="2378" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2378" s="50"/>
-      <c r="N2378" s="47"/>
-      <c r="V2378" s="47"/>
-    </row>
-    <row r="2379" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2379" s="50"/>
-      <c r="N2379" s="47"/>
-      <c r="V2379" s="47"/>
-    </row>
-    <row r="2380" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2380" s="50"/>
-      <c r="N2380" s="47"/>
-      <c r="V2380" s="47"/>
-    </row>
-    <row r="2381" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2381" s="50"/>
-      <c r="N2381" s="47"/>
-      <c r="V2381" s="47"/>
-    </row>
-    <row r="2382" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2382" s="50"/>
-      <c r="N2382" s="47"/>
-      <c r="V2382" s="47"/>
-    </row>
-    <row r="2383" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2383" s="50"/>
-      <c r="N2383" s="47"/>
-      <c r="V2383" s="47"/>
-    </row>
-    <row r="2384" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2384" s="50"/>
-      <c r="N2384" s="47"/>
-      <c r="V2384" s="47"/>
-    </row>
-    <row r="2385" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2385" s="50"/>
-      <c r="N2385" s="47"/>
-      <c r="V2385" s="47"/>
-    </row>
-    <row r="2386" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2386" s="50"/>
-      <c r="N2386" s="47"/>
-      <c r="V2386" s="47"/>
-    </row>
-    <row r="2387" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2387" s="50"/>
-      <c r="N2387" s="47"/>
-      <c r="V2387" s="47"/>
-    </row>
-    <row r="2388" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2388" s="50"/>
-      <c r="N2388" s="47"/>
-      <c r="V2388" s="47"/>
-    </row>
-    <row r="2389" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2389" s="50"/>
-      <c r="N2389" s="47"/>
-      <c r="V2389" s="47"/>
-    </row>
-    <row r="2390" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2390" s="50"/>
-      <c r="N2390" s="47"/>
-      <c r="V2390" s="47"/>
-    </row>
-    <row r="2391" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2391" s="50"/>
-      <c r="N2391" s="47"/>
-      <c r="V2391" s="47"/>
-    </row>
-    <row r="2392" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2392" s="50"/>
-      <c r="N2392" s="47"/>
-      <c r="V2392" s="47"/>
-    </row>
-    <row r="2393" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2393" s="50"/>
-      <c r="N2393" s="47"/>
-      <c r="V2393" s="47"/>
-    </row>
-    <row r="2394" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2394" s="50"/>
-      <c r="N2394" s="47"/>
-      <c r="V2394" s="47"/>
-    </row>
-    <row r="2395" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2395" s="50"/>
-      <c r="N2395" s="47"/>
-      <c r="V2395" s="47"/>
-    </row>
-    <row r="2396" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2396" s="50"/>
-      <c r="N2396" s="47"/>
-      <c r="V2396" s="47"/>
-    </row>
-    <row r="2397" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2397" s="50"/>
-      <c r="N2397" s="47"/>
-      <c r="V2397" s="47"/>
-    </row>
-    <row r="2398" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2398" s="50"/>
-      <c r="N2398" s="47"/>
-      <c r="V2398" s="47"/>
-    </row>
-    <row r="2399" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2399" s="50"/>
-      <c r="N2399" s="47"/>
-      <c r="V2399" s="47"/>
-    </row>
-    <row r="2400" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2400" s="50"/>
-      <c r="N2400" s="47"/>
-      <c r="V2400" s="47"/>
-    </row>
-    <row r="2401" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2401" s="50"/>
-      <c r="N2401" s="47"/>
-      <c r="V2401" s="47"/>
-    </row>
-    <row r="2402" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2402" s="50"/>
-      <c r="N2402" s="47"/>
-      <c r="V2402" s="47"/>
-    </row>
-    <row r="2403" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2403" s="50"/>
-      <c r="N2403" s="47"/>
-      <c r="V2403" s="47"/>
-    </row>
-    <row r="2404" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2404" s="50"/>
-      <c r="N2404" s="47"/>
-      <c r="V2404" s="47"/>
-    </row>
-    <row r="2405" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2405" s="50"/>
-      <c r="N2405" s="47"/>
-      <c r="V2405" s="47"/>
-    </row>
-    <row r="2406" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2406" s="50"/>
-      <c r="N2406" s="47"/>
-      <c r="V2406" s="47"/>
-    </row>
-    <row r="2407" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2407" s="50"/>
-      <c r="N2407" s="47"/>
-      <c r="V2407" s="47"/>
-    </row>
-    <row r="2408" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2408" s="50"/>
-      <c r="N2408" s="47"/>
-      <c r="V2408" s="47"/>
-    </row>
-    <row r="2409" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2409" s="50"/>
-      <c r="N2409" s="47"/>
-      <c r="V2409" s="47"/>
-    </row>
-    <row r="2410" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2410" s="50"/>
-      <c r="N2410" s="47"/>
-      <c r="V2410" s="47"/>
-    </row>
-    <row r="2411" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2411" s="50"/>
-      <c r="N2411" s="47"/>
-      <c r="V2411" s="47"/>
-    </row>
-    <row r="2412" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2412" s="50"/>
-      <c r="N2412" s="47"/>
-      <c r="V2412" s="47"/>
-    </row>
-    <row r="2413" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2413" s="50"/>
-      <c r="N2413" s="47"/>
-      <c r="V2413" s="47"/>
-    </row>
-    <row r="2414" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2414" s="50"/>
-      <c r="N2414" s="47"/>
-      <c r="V2414" s="47"/>
-    </row>
-    <row r="2415" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2415" s="50"/>
-      <c r="N2415" s="47"/>
-      <c r="V2415" s="47"/>
-    </row>
-    <row r="2416" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2416" s="50"/>
-      <c r="N2416" s="47"/>
-      <c r="V2416" s="47"/>
-    </row>
-    <row r="2417" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2417" s="50"/>
-      <c r="N2417" s="47"/>
-      <c r="V2417" s="47"/>
-    </row>
-    <row r="2418" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2418" s="50"/>
-      <c r="N2418" s="47"/>
-      <c r="V2418" s="47"/>
-    </row>
-    <row r="2419" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2419" s="50"/>
-      <c r="N2419" s="47"/>
-      <c r="V2419" s="47"/>
-    </row>
-    <row r="2420" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2420" s="50"/>
-      <c r="N2420" s="47"/>
-      <c r="V2420" s="47"/>
-    </row>
-    <row r="2421" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2421" s="50"/>
-      <c r="N2421" s="47"/>
-      <c r="V2421" s="47"/>
-    </row>
-    <row r="2422" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2422" s="50"/>
-      <c r="N2422" s="47"/>
-      <c r="V2422" s="47"/>
-    </row>
-    <row r="2423" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2423" s="50"/>
-      <c r="N2423" s="47"/>
-      <c r="V2423" s="47"/>
-    </row>
-    <row r="2424" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2424" s="50"/>
-      <c r="N2424" s="47"/>
-      <c r="V2424" s="47"/>
-    </row>
-    <row r="2425" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2425" s="50"/>
-      <c r="N2425" s="47"/>
-      <c r="V2425" s="47"/>
-    </row>
-    <row r="2426" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2426" s="50"/>
-      <c r="N2426" s="47"/>
-      <c r="V2426" s="47"/>
-    </row>
-    <row r="2427" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2427" s="50"/>
-      <c r="N2427" s="47"/>
-      <c r="V2427" s="47"/>
-    </row>
-    <row r="2428" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2428" s="50"/>
-      <c r="N2428" s="47"/>
-      <c r="V2428" s="47"/>
-    </row>
-    <row r="2429" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2429" s="50"/>
-      <c r="N2429" s="47"/>
-      <c r="V2429" s="47"/>
-    </row>
-    <row r="2430" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2430" s="50"/>
-      <c r="N2430" s="47"/>
-      <c r="V2430" s="47"/>
-    </row>
-    <row r="2431" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2431" s="50"/>
-      <c r="N2431" s="47"/>
-      <c r="V2431" s="47"/>
-    </row>
-    <row r="2432" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2432" s="50"/>
-      <c r="N2432" s="47"/>
-      <c r="V2432" s="47"/>
-    </row>
-    <row r="2433" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2433" s="50"/>
-      <c r="N2433" s="47"/>
-      <c r="V2433" s="47"/>
-    </row>
-    <row r="2434" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2434" s="50"/>
-      <c r="N2434" s="47"/>
-      <c r="V2434" s="47"/>
-    </row>
-    <row r="2435" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2435" s="50"/>
-      <c r="N2435" s="47"/>
-      <c r="V2435" s="47"/>
-    </row>
-    <row r="2436" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2436" s="50"/>
-      <c r="N2436" s="47"/>
-      <c r="V2436" s="47"/>
-    </row>
-    <row r="2437" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2437" s="50"/>
-      <c r="N2437" s="47"/>
-      <c r="V2437" s="47"/>
-    </row>
-    <row r="2438" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2438" s="50"/>
-      <c r="N2438" s="47"/>
-      <c r="V2438" s="47"/>
-    </row>
-    <row r="2439" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2439" s="50"/>
-      <c r="N2439" s="47"/>
-      <c r="V2439" s="47"/>
-    </row>
-    <row r="2440" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2440" s="50"/>
-      <c r="N2440" s="47"/>
-      <c r="V2440" s="47"/>
-    </row>
-    <row r="2441" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2441" s="50"/>
-      <c r="N2441" s="47"/>
-      <c r="V2441" s="47"/>
-    </row>
-    <row r="2442" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2442" s="50"/>
-      <c r="N2442" s="47"/>
-      <c r="V2442" s="47"/>
-    </row>
-    <row r="2443" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2443" s="50"/>
-      <c r="N2443" s="47"/>
-      <c r="V2443" s="47"/>
-    </row>
-    <row r="2444" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2444" s="50"/>
-      <c r="N2444" s="47"/>
-      <c r="V2444" s="47"/>
-    </row>
-    <row r="2445" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2445" s="50"/>
-      <c r="N2445" s="47"/>
-      <c r="V2445" s="47"/>
-    </row>
-    <row r="2446" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2446" s="50"/>
-      <c r="N2446" s="47"/>
-      <c r="V2446" s="47"/>
-    </row>
-    <row r="2447" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2447" s="50"/>
-      <c r="N2447" s="47"/>
-      <c r="V2447" s="47"/>
-    </row>
-    <row r="2448" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2448" s="50"/>
-      <c r="N2448" s="47"/>
-      <c r="V2448" s="47"/>
-    </row>
-    <row r="2449" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2449" s="50"/>
-      <c r="N2449" s="47"/>
-      <c r="V2449" s="47"/>
-    </row>
-    <row r="2450" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2450" s="50"/>
-      <c r="N2450" s="47"/>
-      <c r="V2450" s="47"/>
-    </row>
-    <row r="2451" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2451" s="50"/>
-      <c r="N2451" s="47"/>
-      <c r="V2451" s="47"/>
-    </row>
-    <row r="2452" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2452" s="50"/>
-      <c r="N2452" s="48"/>
-      <c r="V2452" s="48"/>
-    </row>
-    <row r="2453" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2453" s="50"/>
-      <c r="N2453" s="47"/>
-      <c r="V2453" s="47"/>
-    </row>
-    <row r="2454" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2454" s="50"/>
-      <c r="N2454" s="47"/>
-      <c r="V2454" s="47"/>
-    </row>
-    <row r="2455" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2455" s="50"/>
-      <c r="N2455" s="47"/>
-      <c r="V2455" s="47"/>
-    </row>
-    <row r="2456" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2456" s="50"/>
-      <c r="N2456" s="47"/>
-      <c r="V2456" s="47"/>
-    </row>
-    <row r="2457" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2457" s="50"/>
-      <c r="N2457" s="47"/>
-      <c r="V2457" s="47"/>
-    </row>
-    <row r="2458" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2458" s="50"/>
-      <c r="N2458" s="47"/>
-      <c r="V2458" s="47"/>
-    </row>
-    <row r="2459" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2459" s="50"/>
-      <c r="N2459" s="47"/>
-      <c r="V2459" s="47"/>
-    </row>
-    <row r="2460" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2460" s="50"/>
-      <c r="N2460" s="47"/>
-      <c r="V2460" s="47"/>
-    </row>
-    <row r="2461" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2461" s="50"/>
-      <c r="N2461" s="47"/>
-      <c r="V2461" s="47"/>
-    </row>
-    <row r="2462" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2462" s="50"/>
-      <c r="N2462" s="47"/>
-      <c r="V2462" s="47"/>
-    </row>
-    <row r="2463" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2463" s="50"/>
-      <c r="N2463" s="47"/>
-      <c r="V2463" s="47"/>
-    </row>
-    <row r="2464" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2464" s="50"/>
-      <c r="N2464" s="47"/>
-      <c r="V2464" s="47"/>
-    </row>
-    <row r="2465" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2465" s="50"/>
-      <c r="N2465" s="47"/>
-      <c r="V2465" s="47"/>
-    </row>
-    <row r="2466" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2466" s="50"/>
-      <c r="N2466" s="47"/>
-      <c r="V2466" s="47"/>
-    </row>
-    <row r="2467" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2467" s="50"/>
-      <c r="N2467" s="47"/>
-      <c r="V2467" s="47"/>
-    </row>
-    <row r="2468" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2468" s="50"/>
-      <c r="N2468" s="47"/>
-      <c r="V2468" s="47"/>
-    </row>
-    <row r="2469" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2469" s="50"/>
-      <c r="N2469" s="47"/>
-      <c r="V2469" s="47"/>
-    </row>
-    <row r="2470" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2470" s="50"/>
-      <c r="N2470" s="47"/>
-      <c r="V2470" s="47"/>
-    </row>
-    <row r="2471" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2471" s="50"/>
-      <c r="N2471" s="47"/>
-      <c r="V2471" s="47"/>
-    </row>
-    <row r="2472" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2472" s="50"/>
-      <c r="N2472" s="47"/>
-      <c r="V2472" s="47"/>
-    </row>
-    <row r="2473" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2473" s="50"/>
-      <c r="N2473" s="47"/>
-      <c r="V2473" s="47"/>
-    </row>
-    <row r="2474" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2474" s="50"/>
-      <c r="N2474" s="47"/>
-      <c r="V2474" s="47"/>
-    </row>
-    <row r="2475" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2475" s="50"/>
-      <c r="N2475" s="47"/>
-      <c r="V2475" s="47"/>
-    </row>
-    <row r="2476" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2476" s="50"/>
-      <c r="N2476" s="47"/>
-      <c r="V2476" s="47"/>
-    </row>
-    <row r="2477" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2477" s="50"/>
-      <c r="N2477" s="47"/>
-      <c r="V2477" s="47"/>
-    </row>
-    <row r="2478" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2478" s="50"/>
-      <c r="N2478" s="47"/>
-      <c r="V2478" s="47"/>
-    </row>
-    <row r="2479" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2479" s="50"/>
-      <c r="N2479" s="47"/>
-      <c r="V2479" s="47"/>
-    </row>
-    <row r="2480" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2480" s="50"/>
-      <c r="N2480" s="47"/>
-      <c r="V2480" s="47"/>
-    </row>
-    <row r="2481" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2481" s="50"/>
-      <c r="N2481" s="47"/>
-      <c r="V2481" s="47"/>
-    </row>
-    <row r="2482" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2482" s="50"/>
-      <c r="N2482" s="47"/>
-      <c r="V2482" s="47"/>
-    </row>
-    <row r="2483" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2483" s="50"/>
-      <c r="N2483" s="47"/>
-      <c r="V2483" s="47"/>
-    </row>
-    <row r="2484" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2484" s="50"/>
-      <c r="N2484" s="47"/>
-      <c r="V2484" s="47"/>
-    </row>
-    <row r="2485" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2485" s="50"/>
-      <c r="N2485" s="47"/>
-      <c r="V2485" s="47"/>
-    </row>
-    <row r="2486" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2486" s="50"/>
-      <c r="N2486" s="47"/>
-      <c r="V2486" s="47"/>
-    </row>
-    <row r="2487" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2487" s="50"/>
-      <c r="N2487" s="47"/>
-      <c r="V2487" s="47"/>
-    </row>
-    <row r="2488" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2488" s="50"/>
-      <c r="N2488" s="47"/>
-      <c r="V2488" s="47"/>
-    </row>
-    <row r="2489" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2489" s="50"/>
-      <c r="N2489" s="47"/>
-      <c r="V2489" s="47"/>
-    </row>
-    <row r="2490" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2490" s="50"/>
-      <c r="N2490" s="47"/>
-      <c r="V2490" s="47"/>
-    </row>
-    <row r="2491" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2491" s="50"/>
-      <c r="N2491" s="47"/>
-      <c r="V2491" s="47"/>
-    </row>
-    <row r="2492" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2492" s="50"/>
-      <c r="N2492" s="47"/>
-      <c r="V2492" s="47"/>
-    </row>
-    <row r="2493" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2493" s="50"/>
-      <c r="N2493" s="47"/>
-      <c r="V2493" s="47"/>
-    </row>
-    <row r="2494" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2494" s="50"/>
-      <c r="N2494" s="47"/>
-      <c r="V2494" s="47"/>
-    </row>
-    <row r="2495" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2495" s="50"/>
-      <c r="N2495" s="47"/>
-      <c r="V2495" s="47"/>
-    </row>
-    <row r="2496" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2496" s="50"/>
-      <c r="N2496" s="47"/>
-      <c r="V2496" s="47"/>
-    </row>
-    <row r="2497" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2497" s="50"/>
-      <c r="N2497" s="47"/>
-      <c r="V2497" s="47"/>
-    </row>
-    <row r="2498" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2498" s="50"/>
-      <c r="N2498" s="47"/>
-      <c r="V2498" s="47"/>
-    </row>
-    <row r="2499" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2499" s="50"/>
-      <c r="N2499" s="47"/>
-      <c r="V2499" s="47"/>
-    </row>
-    <row r="2500" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2500" s="50"/>
-      <c r="N2500" s="47"/>
-      <c r="V2500" s="47"/>
-    </row>
-    <row r="2501" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2501" s="50"/>
-      <c r="N2501" s="47"/>
-      <c r="V2501" s="47"/>
-    </row>
-    <row r="2502" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2502" s="50"/>
-      <c r="N2502" s="47"/>
-      <c r="V2502" s="47"/>
-    </row>
-    <row r="2503" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2503" s="50"/>
-      <c r="N2503" s="47"/>
-      <c r="V2503" s="47"/>
-    </row>
-    <row r="2504" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2504" s="50"/>
-      <c r="N2504" s="47"/>
-      <c r="V2504" s="47"/>
-    </row>
-    <row r="2505" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2505" s="50"/>
-      <c r="N2505" s="47"/>
-      <c r="V2505" s="47"/>
-    </row>
-    <row r="2506" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2506" s="50"/>
-      <c r="N2506" s="47"/>
-      <c r="V2506" s="47"/>
-    </row>
-    <row r="2507" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2507" s="50"/>
-      <c r="N2507" s="47"/>
-      <c r="V2507" s="47"/>
-    </row>
-    <row r="2508" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2508" s="50"/>
-      <c r="N2508" s="47"/>
-      <c r="V2508" s="47"/>
-    </row>
-    <row r="2509" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2509" s="50"/>
-      <c r="N2509" s="47"/>
-      <c r="V2509" s="47"/>
-    </row>
-    <row r="2510" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2510" s="50"/>
-      <c r="N2510" s="47"/>
-      <c r="V2510" s="47"/>
-    </row>
-    <row r="2511" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2511" s="50"/>
-      <c r="N2511" s="47"/>
-      <c r="V2511" s="47"/>
-    </row>
-    <row r="2512" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2512" s="50"/>
-      <c r="N2512" s="47"/>
-      <c r="V2512" s="47"/>
-    </row>
-    <row r="2513" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2513" s="50"/>
-      <c r="N2513" s="47"/>
-      <c r="V2513" s="47"/>
-    </row>
-    <row r="2514" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2514" s="50"/>
-      <c r="N2514" s="47"/>
-      <c r="V2514" s="47"/>
-    </row>
-    <row r="2515" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2515" s="50"/>
-      <c r="N2515" s="47"/>
-      <c r="V2515" s="47"/>
-    </row>
-    <row r="2516" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2516" s="50"/>
-      <c r="N2516" s="47"/>
-      <c r="V2516" s="47"/>
-    </row>
-    <row r="2517" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2517" s="50"/>
-      <c r="N2517" s="47"/>
-      <c r="V2517" s="47"/>
-    </row>
-    <row r="2518" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2518" s="50"/>
-      <c r="N2518" s="47"/>
-      <c r="V2518" s="47"/>
-    </row>
-    <row r="2519" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2519" s="50"/>
-      <c r="N2519" s="47"/>
-      <c r="V2519" s="47"/>
-    </row>
-    <row r="2520" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2520" s="50"/>
-      <c r="N2520" s="47"/>
-      <c r="V2520" s="47"/>
-    </row>
-    <row r="2521" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2521" s="50"/>
-      <c r="N2521" s="47"/>
-      <c r="V2521" s="47"/>
-    </row>
-    <row r="2522" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2522" s="50"/>
-      <c r="N2522" s="47"/>
-      <c r="V2522" s="47"/>
-    </row>
-    <row r="2523" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2523" s="50"/>
-      <c r="N2523" s="47"/>
-      <c r="V2523" s="47"/>
-    </row>
-    <row r="2524" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2524" s="50"/>
-      <c r="N2524" s="47"/>
-      <c r="V2524" s="47"/>
-    </row>
-    <row r="2525" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2525" s="50"/>
-      <c r="N2525" s="47"/>
-      <c r="V2525" s="47"/>
-    </row>
-    <row r="2526" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2526" s="50"/>
-      <c r="N2526" s="47"/>
-      <c r="V2526" s="47"/>
-    </row>
-    <row r="2527" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2527" s="50"/>
-      <c r="N2527" s="47"/>
-      <c r="V2527" s="47"/>
-    </row>
-    <row r="2528" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2528" s="50"/>
-      <c r="N2528" s="47"/>
-      <c r="V2528" s="47"/>
-    </row>
-    <row r="2529" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2529" s="50"/>
-      <c r="N2529" s="47"/>
-      <c r="V2529" s="47"/>
-    </row>
-    <row r="2530" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2530" s="50"/>
-      <c r="N2530" s="47"/>
-      <c r="V2530" s="47"/>
-    </row>
-    <row r="2531" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2531" s="50"/>
-      <c r="N2531" s="47"/>
-      <c r="V2531" s="47"/>
-    </row>
-    <row r="2532" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2532" s="50"/>
-      <c r="N2532" s="47"/>
-      <c r="V2532" s="47"/>
-    </row>
-    <row r="2533" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2533" s="50"/>
-      <c r="N2533" s="47"/>
-      <c r="V2533" s="47"/>
-    </row>
-    <row r="2534" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2534" s="50"/>
-      <c r="N2534" s="47"/>
-      <c r="V2534" s="47"/>
-    </row>
-    <row r="2535" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2535" s="50"/>
-      <c r="N2535" s="47"/>
-      <c r="V2535" s="47"/>
-    </row>
-    <row r="2536" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2536" s="50"/>
-      <c r="N2536" s="47"/>
-      <c r="V2536" s="47"/>
-    </row>
-    <row r="2537" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2537" s="50"/>
-      <c r="N2537" s="47"/>
-      <c r="V2537" s="47"/>
-    </row>
-    <row r="2538" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2538" s="50"/>
-      <c r="N2538" s="47"/>
-      <c r="V2538" s="47"/>
-    </row>
-    <row r="2539" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2539" s="50"/>
-      <c r="N2539" s="47"/>
-      <c r="V2539" s="47"/>
-    </row>
-    <row r="2540" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2540" s="50"/>
-      <c r="N2540" s="47"/>
-      <c r="V2540" s="47"/>
-    </row>
-    <row r="2541" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2541" s="50"/>
-      <c r="N2541" s="47"/>
-      <c r="V2541" s="47"/>
-    </row>
-    <row r="2542" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2542" s="50"/>
-      <c r="N2542" s="47"/>
-      <c r="V2542" s="47"/>
-    </row>
-    <row r="2543" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2543" s="50"/>
-      <c r="N2543" s="47"/>
-      <c r="V2543" s="47"/>
-    </row>
-    <row r="2544" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2544" s="50"/>
-      <c r="N2544" s="47"/>
-      <c r="V2544" s="47"/>
-    </row>
-    <row r="2545" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2545" s="50"/>
-      <c r="N2545" s="47"/>
-      <c r="V2545" s="47"/>
-    </row>
-    <row r="2546" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2546" s="50"/>
-      <c r="N2546" s="47"/>
-      <c r="V2546" s="47"/>
-    </row>
-    <row r="2547" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2547" s="50"/>
-      <c r="N2547" s="47"/>
-      <c r="V2547" s="47"/>
-    </row>
-    <row r="2548" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2548" s="50"/>
-      <c r="N2548" s="47"/>
-      <c r="V2548" s="47"/>
-    </row>
-    <row r="2549" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2549" s="50"/>
-      <c r="N2549" s="47"/>
-      <c r="V2549" s="47"/>
-    </row>
-    <row r="2550" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2550" s="50"/>
-      <c r="N2550" s="47"/>
-      <c r="V2550" s="47"/>
-    </row>
-    <row r="2551" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2551" s="50"/>
-      <c r="N2551" s="47"/>
-      <c r="V2551" s="47"/>
-    </row>
-    <row r="2552" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2552" s="50"/>
-      <c r="N2552" s="47"/>
-      <c r="V2552" s="47"/>
-    </row>
-    <row r="2553" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2553" s="50"/>
-      <c r="N2553" s="47"/>
-      <c r="V2553" s="47"/>
-    </row>
-    <row r="2554" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2554" s="50"/>
-      <c r="N2554" s="47"/>
-      <c r="V2554" s="47"/>
-    </row>
-    <row r="2555" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2555" s="50"/>
-      <c r="N2555" s="47"/>
-      <c r="V2555" s="47"/>
-    </row>
-    <row r="2556" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2556" s="50"/>
-      <c r="N2556" s="47"/>
-      <c r="V2556" s="47"/>
-    </row>
-    <row r="2557" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2557" s="50"/>
-      <c r="N2557" s="47"/>
-      <c r="V2557" s="47"/>
-    </row>
-    <row r="2558" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2558" s="50"/>
-      <c r="N2558" s="47"/>
-      <c r="V2558" s="47"/>
-    </row>
-    <row r="2559" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2559" s="50"/>
-      <c r="N2559" s="47"/>
-      <c r="V2559" s="47"/>
-    </row>
-    <row r="2560" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2560" s="50"/>
-      <c r="N2560" s="47"/>
-      <c r="V2560" s="47"/>
-    </row>
-    <row r="2561" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2561" s="50"/>
-      <c r="N2561" s="47"/>
-      <c r="V2561" s="47"/>
-    </row>
-    <row r="2562" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2562" s="50"/>
-      <c r="N2562" s="47"/>
-      <c r="V2562" s="47"/>
-    </row>
-    <row r="2563" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2563" s="50"/>
-      <c r="N2563" s="47"/>
-      <c r="V2563" s="47"/>
-    </row>
-    <row r="2564" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2564" s="50"/>
-      <c r="N2564" s="47"/>
-      <c r="V2564" s="47"/>
-    </row>
-    <row r="2565" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2565" s="50"/>
-      <c r="N2565" s="47"/>
-      <c r="V2565" s="47"/>
-    </row>
-    <row r="2566" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2566" s="50"/>
-      <c r="N2566" s="47"/>
-      <c r="V2566" s="47"/>
-    </row>
-    <row r="2567" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2567" s="50"/>
-      <c r="N2567" s="47"/>
-      <c r="V2567" s="47"/>
-    </row>
-    <row r="2568" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2568" s="50"/>
-      <c r="N2568" s="47"/>
-      <c r="V2568" s="47"/>
-    </row>
-    <row r="2569" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2569" s="50"/>
-      <c r="N2569" s="47"/>
-      <c r="V2569" s="47"/>
-    </row>
-    <row r="2570" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2570" s="50"/>
-      <c r="N2570" s="47"/>
-      <c r="V2570" s="47"/>
-    </row>
-    <row r="2571" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2571" s="50"/>
-      <c r="N2571" s="47"/>
-      <c r="V2571" s="47"/>
-    </row>
-    <row r="2572" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2572" s="50"/>
-      <c r="N2572" s="47"/>
-      <c r="V2572" s="47"/>
-    </row>
-    <row r="2573" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2573" s="50"/>
-      <c r="N2573" s="47"/>
-      <c r="V2573" s="47"/>
-    </row>
-    <row r="2574" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2574" s="50"/>
-      <c r="N2574" s="47"/>
-      <c r="V2574" s="47"/>
-    </row>
-    <row r="2575" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2575" s="50"/>
-      <c r="N2575" s="47"/>
-      <c r="V2575" s="47"/>
-    </row>
-    <row r="2576" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2576" s="50"/>
-      <c r="N2576" s="47"/>
-      <c r="V2576" s="47"/>
-    </row>
-    <row r="2577" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2577" s="50"/>
-      <c r="N2577" s="47"/>
-      <c r="V2577" s="47"/>
-    </row>
-    <row r="2578" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2578" s="50"/>
-      <c r="N2578" s="47"/>
-      <c r="V2578" s="47"/>
-    </row>
-    <row r="2579" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2579" s="50"/>
-      <c r="N2579" s="47"/>
-      <c r="V2579" s="47"/>
-    </row>
-    <row r="2580" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2580" s="50"/>
-      <c r="N2580" s="47"/>
-      <c r="V2580" s="47"/>
-    </row>
-    <row r="2581" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2581" s="50"/>
-      <c r="N2581" s="47"/>
-      <c r="V2581" s="47"/>
-    </row>
-    <row r="2582" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2582" s="50"/>
-      <c r="N2582" s="47"/>
-      <c r="V2582" s="47"/>
-    </row>
-    <row r="2583" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2583" s="50"/>
-      <c r="N2583" s="47"/>
-      <c r="V2583" s="47"/>
-    </row>
-    <row r="2584" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2584" s="50"/>
-      <c r="N2584" s="47"/>
-      <c r="V2584" s="47"/>
-    </row>
-    <row r="2585" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2585" s="50"/>
-      <c r="N2585" s="47"/>
-      <c r="V2585" s="47"/>
-    </row>
-    <row r="2586" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2586" s="50"/>
-      <c r="N2586" s="47"/>
-      <c r="V2586" s="47"/>
-    </row>
-    <row r="2587" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2587" s="50"/>
-      <c r="N2587" s="47"/>
-      <c r="V2587" s="47"/>
-    </row>
-    <row r="2588" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2588" s="50"/>
-      <c r="N2588" s="47"/>
-      <c r="V2588" s="47"/>
-    </row>
-    <row r="2589" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2589" s="50"/>
-      <c r="N2589" s="47"/>
-      <c r="V2589" s="47"/>
-    </row>
-    <row r="2590" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2590" s="50"/>
-      <c r="N2590" s="47"/>
-      <c r="V2590" s="47"/>
-    </row>
-    <row r="2591" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2591" s="50"/>
-      <c r="N2591" s="47"/>
-      <c r="V2591" s="47"/>
-    </row>
-    <row r="2592" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2592" s="50"/>
-      <c r="N2592" s="47"/>
-      <c r="V2592" s="47"/>
-    </row>
-    <row r="2593" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2593" s="50"/>
-      <c r="N2593" s="47"/>
-      <c r="V2593" s="47"/>
-    </row>
-    <row r="2594" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2594" s="50"/>
-      <c r="N2594" s="47"/>
-      <c r="V2594" s="47"/>
-    </row>
-    <row r="2595" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2595" s="50"/>
-      <c r="N2595" s="47"/>
-      <c r="V2595" s="47"/>
-    </row>
-    <row r="2596" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2596" s="50"/>
-      <c r="N2596" s="47"/>
-      <c r="V2596" s="47"/>
-    </row>
-    <row r="2597" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2597" s="50"/>
-      <c r="N2597" s="47"/>
-      <c r="V2597" s="47"/>
-    </row>
-    <row r="2598" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2598" s="50"/>
-      <c r="N2598" s="47"/>
-      <c r="V2598" s="47"/>
-    </row>
-    <row r="2599" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2599" s="50"/>
-      <c r="N2599" s="47"/>
-      <c r="V2599" s="47"/>
-    </row>
-    <row r="2600" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2600" s="50"/>
-      <c r="N2600" s="47"/>
-      <c r="V2600" s="47"/>
-    </row>
-    <row r="2601" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2601" s="50"/>
-      <c r="N2601" s="47"/>
-      <c r="V2601" s="47"/>
-    </row>
-    <row r="2602" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2602" s="50"/>
-      <c r="N2602" s="47"/>
-      <c r="V2602" s="47"/>
-    </row>
-    <row r="2603" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2603" s="50"/>
-      <c r="N2603" s="47"/>
-      <c r="V2603" s="47"/>
-    </row>
-    <row r="2604" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2604" s="50"/>
-      <c r="N2604" s="47"/>
-      <c r="V2604" s="47"/>
-    </row>
-    <row r="2605" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2605" s="50"/>
-      <c r="N2605" s="47"/>
-      <c r="V2605" s="47"/>
-    </row>
-    <row r="2606" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2606" s="50"/>
-      <c r="N2606" s="47"/>
-      <c r="V2606" s="47"/>
-    </row>
-    <row r="2607" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2607" s="50"/>
-      <c r="N2607" s="47"/>
-      <c r="V2607" s="47"/>
-    </row>
-    <row r="2608" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2608" s="50"/>
-      <c r="N2608" s="47"/>
-      <c r="V2608" s="47"/>
-    </row>
-    <row r="2609" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2609" s="50"/>
-      <c r="N2609" s="47"/>
-      <c r="V2609" s="47"/>
-    </row>
-    <row r="2610" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2610" s="50"/>
-      <c r="N2610" s="47"/>
-      <c r="V2610" s="47"/>
-    </row>
-    <row r="2611" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2611" s="50"/>
-      <c r="N2611" s="47"/>
-      <c r="V2611" s="47"/>
-    </row>
-    <row r="2612" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2612" s="50"/>
-      <c r="N2612" s="47"/>
-      <c r="V2612" s="47"/>
-    </row>
-    <row r="2613" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2613" s="50"/>
-      <c r="N2613" s="47"/>
-      <c r="V2613" s="47"/>
-    </row>
-    <row r="2614" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2614" s="50"/>
-      <c r="N2614" s="47"/>
-      <c r="V2614" s="47"/>
-    </row>
-    <row r="2615" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2615" s="50"/>
-      <c r="N2615" s="47"/>
-      <c r="V2615" s="47"/>
-    </row>
-    <row r="2616" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2616" s="50"/>
-      <c r="N2616" s="47"/>
-      <c r="V2616" s="47"/>
-    </row>
-    <row r="2617" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2617" s="50"/>
-      <c r="N2617" s="47"/>
-      <c r="V2617" s="47"/>
-    </row>
-    <row r="2618" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2618" s="50"/>
-      <c r="N2618" s="47"/>
-      <c r="V2618" s="47"/>
-    </row>
-    <row r="2619" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2619" s="50"/>
-      <c r="N2619" s="47"/>
-      <c r="V2619" s="47"/>
-    </row>
-    <row r="2620" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2620" s="50"/>
-      <c r="N2620" s="47"/>
-      <c r="V2620" s="47"/>
-    </row>
-    <row r="2621" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2621" s="50"/>
-      <c r="N2621" s="47"/>
-      <c r="V2621" s="47"/>
-    </row>
-    <row r="2622" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2622" s="50"/>
-      <c r="N2622" s="47"/>
-      <c r="V2622" s="47"/>
-    </row>
-    <row r="2623" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2623" s="50"/>
-      <c r="N2623" s="47"/>
-      <c r="V2623" s="47"/>
-    </row>
-    <row r="2624" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2624" s="50"/>
-      <c r="N2624" s="47"/>
-      <c r="V2624" s="47"/>
-    </row>
-    <row r="2625" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2625" s="50"/>
-      <c r="N2625" s="47"/>
-      <c r="V2625" s="47"/>
-    </row>
-    <row r="2626" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2626" s="50"/>
-      <c r="N2626" s="47"/>
-      <c r="V2626" s="47"/>
-    </row>
-    <row r="2627" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2627" s="50"/>
-      <c r="N2627" s="47"/>
-      <c r="V2627" s="47"/>
-    </row>
-    <row r="2628" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2628" s="50"/>
-      <c r="N2628" s="47"/>
-      <c r="V2628" s="47"/>
-    </row>
-    <row r="2629" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2629" s="50"/>
-      <c r="N2629" s="47"/>
-      <c r="V2629" s="47"/>
-    </row>
-    <row r="2630" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2630" s="50"/>
-      <c r="N2630" s="47"/>
-      <c r="V2630" s="47"/>
-    </row>
-    <row r="2631" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2631" s="50"/>
-      <c r="N2631" s="47"/>
-      <c r="V2631" s="47"/>
-    </row>
-    <row r="2632" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2632" s="50"/>
-      <c r="N2632" s="47"/>
-      <c r="V2632" s="47"/>
-    </row>
-    <row r="2633" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2633" s="50"/>
-      <c r="N2633" s="47"/>
-      <c r="V2633" s="47"/>
-    </row>
-    <row r="2634" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2634" s="50"/>
-      <c r="N2634" s="47"/>
-      <c r="V2634" s="47"/>
-    </row>
-    <row r="2635" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2635" s="50"/>
-      <c r="N2635" s="47"/>
-      <c r="V2635" s="47"/>
-    </row>
-    <row r="2636" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2636" s="50"/>
-      <c r="N2636" s="47"/>
-      <c r="V2636" s="47"/>
-    </row>
-    <row r="2637" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2637" s="50"/>
-      <c r="N2637" s="47"/>
-      <c r="V2637" s="47"/>
-    </row>
-    <row r="2638" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2638" s="50"/>
-      <c r="N2638" s="47"/>
-      <c r="V2638" s="47"/>
-    </row>
-    <row r="2639" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2639" s="50"/>
-      <c r="N2639" s="47"/>
-      <c r="V2639" s="47"/>
-    </row>
-    <row r="2640" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2640" s="50"/>
-      <c r="N2640" s="47"/>
-      <c r="V2640" s="47"/>
-    </row>
-    <row r="2641" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2641" s="50"/>
-      <c r="N2641" s="47"/>
-      <c r="V2641" s="47"/>
-    </row>
-    <row r="2642" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2642" s="50"/>
-      <c r="N2642" s="47"/>
-      <c r="V2642" s="47"/>
-    </row>
-    <row r="2643" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2643" s="50"/>
-      <c r="N2643" s="47"/>
-      <c r="V2643" s="47"/>
-    </row>
-    <row r="2644" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2644" s="50"/>
-      <c r="N2644" s="47"/>
-      <c r="V2644" s="47"/>
-    </row>
-    <row r="2645" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2645" s="50"/>
-      <c r="N2645" s="47"/>
-      <c r="V2645" s="47"/>
-    </row>
-    <row r="2646" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2646" s="50"/>
-      <c r="N2646" s="47"/>
-      <c r="V2646" s="47"/>
-    </row>
-    <row r="2647" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2647" s="50"/>
-      <c r="N2647" s="47"/>
-      <c r="V2647" s="47"/>
-    </row>
-    <row r="2648" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2648" s="50"/>
-      <c r="N2648" s="47"/>
-      <c r="V2648" s="47"/>
-    </row>
-    <row r="2649" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2649" s="50"/>
-      <c r="N2649" s="47"/>
-      <c r="V2649" s="47"/>
-    </row>
-    <row r="2650" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2650" s="50"/>
-      <c r="N2650" s="47"/>
-      <c r="V2650" s="47"/>
-    </row>
-    <row r="2651" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2651" s="50"/>
-      <c r="N2651" s="47"/>
-      <c r="V2651" s="47"/>
-    </row>
-    <row r="2652" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2652" s="50"/>
-      <c r="N2652" s="47"/>
-      <c r="V2652" s="47"/>
-    </row>
-    <row r="2653" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2653" s="50"/>
-      <c r="N2653" s="47"/>
-      <c r="V2653" s="47"/>
-    </row>
-    <row r="2654" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2654" s="50"/>
-      <c r="N2654" s="47"/>
-      <c r="V2654" s="47"/>
-    </row>
-    <row r="2655" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2655" s="50"/>
-      <c r="N2655" s="47"/>
-      <c r="V2655" s="47"/>
-    </row>
-    <row r="2656" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2656" s="50"/>
-      <c r="N2656" s="47"/>
-      <c r="V2656" s="47"/>
-    </row>
-    <row r="2657" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2657" s="50"/>
-      <c r="N2657" s="47"/>
-      <c r="V2657" s="47"/>
-    </row>
-    <row r="2658" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2658" s="50"/>
-      <c r="N2658" s="47"/>
-      <c r="V2658" s="47"/>
-    </row>
-    <row r="2659" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2659" s="50"/>
-      <c r="N2659" s="47"/>
-      <c r="V2659" s="47"/>
-    </row>
-    <row r="2660" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2660" s="50"/>
-      <c r="N2660" s="47"/>
-      <c r="V2660" s="47"/>
-    </row>
-    <row r="2661" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2661" s="50"/>
-      <c r="N2661" s="47"/>
-      <c r="V2661" s="47"/>
-    </row>
-    <row r="2662" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2662" s="50"/>
-      <c r="N2662" s="47"/>
-      <c r="V2662" s="47"/>
-    </row>
-    <row r="2663" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2663" s="50"/>
-      <c r="N2663" s="47"/>
-      <c r="V2663" s="47"/>
-    </row>
-    <row r="2664" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2664" s="50"/>
-      <c r="N2664" s="47"/>
-      <c r="V2664" s="47"/>
-    </row>
-    <row r="2665" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2665" s="50"/>
-      <c r="N2665" s="47"/>
-      <c r="V2665" s="47"/>
-    </row>
-    <row r="2666" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2666" s="50"/>
-      <c r="N2666" s="47"/>
-      <c r="V2666" s="47"/>
-    </row>
-    <row r="2667" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2667" s="50"/>
-      <c r="N2667" s="47"/>
-      <c r="V2667" s="47"/>
-    </row>
-    <row r="2668" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2668" s="50"/>
-      <c r="N2668" s="47"/>
-      <c r="V2668" s="47"/>
-    </row>
-    <row r="2669" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2669" s="50"/>
-      <c r="N2669" s="47"/>
-      <c r="V2669" s="47"/>
-    </row>
-    <row r="2670" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2670" s="50"/>
-      <c r="N2670" s="47"/>
-      <c r="V2670" s="47"/>
-    </row>
-    <row r="2671" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2671" s="50"/>
-      <c r="N2671" s="47"/>
-      <c r="V2671" s="47"/>
-    </row>
-    <row r="2672" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2672" s="50"/>
-      <c r="N2672" s="47"/>
-      <c r="V2672" s="47"/>
-    </row>
-    <row r="2673" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2673" s="50"/>
-      <c r="N2673" s="47"/>
-      <c r="V2673" s="47"/>
-    </row>
-    <row r="2674" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2674" s="50"/>
-      <c r="N2674" s="47"/>
-      <c r="V2674" s="47"/>
-    </row>
-    <row r="2675" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2675" s="50"/>
-      <c r="N2675" s="47"/>
-      <c r="V2675" s="47"/>
-    </row>
-    <row r="2676" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2676" s="50"/>
-      <c r="N2676" s="47"/>
-      <c r="V2676" s="47"/>
-    </row>
-    <row r="2677" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2677" s="50"/>
-      <c r="N2677" s="47"/>
-      <c r="V2677" s="47"/>
-    </row>
-    <row r="2678" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2678" s="50"/>
-      <c r="N2678" s="47"/>
-      <c r="V2678" s="47"/>
-    </row>
-    <row r="2679" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2679" s="50"/>
-      <c r="N2679" s="47"/>
-      <c r="V2679" s="47"/>
-    </row>
-    <row r="2680" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2680" s="50"/>
-      <c r="N2680" s="47"/>
-      <c r="V2680" s="47"/>
-    </row>
-    <row r="2681" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2681" s="50"/>
-      <c r="N2681" s="47"/>
-      <c r="V2681" s="47"/>
-    </row>
-    <row r="2682" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2682" s="50"/>
-      <c r="N2682" s="47"/>
-      <c r="V2682" s="47"/>
-    </row>
-    <row r="2683" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2683" s="50"/>
-      <c r="N2683" s="47"/>
-      <c r="V2683" s="47"/>
-    </row>
-    <row r="2684" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2684" s="50"/>
-      <c r="N2684" s="47"/>
-      <c r="V2684" s="47"/>
-    </row>
-    <row r="2685" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2685" s="50"/>
-      <c r="N2685" s="47"/>
-      <c r="V2685" s="47"/>
-    </row>
-    <row r="2686" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2686" s="50"/>
-      <c r="N2686" s="47"/>
-      <c r="V2686" s="47"/>
-    </row>
-    <row r="2687" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2687" s="50"/>
-      <c r="N2687" s="47"/>
-      <c r="V2687" s="47"/>
-    </row>
-    <row r="2688" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2688" s="50"/>
-      <c r="N2688" s="47"/>
-      <c r="V2688" s="47"/>
-    </row>
-    <row r="2689" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2689" s="50"/>
-      <c r="N2689" s="47"/>
-      <c r="V2689" s="47"/>
-    </row>
-    <row r="2690" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2690" s="50"/>
-      <c r="N2690" s="47"/>
-      <c r="V2690" s="47"/>
-    </row>
-    <row r="2691" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2691" s="50"/>
-      <c r="N2691" s="47"/>
-      <c r="V2691" s="47"/>
-    </row>
-    <row r="2692" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2692" s="50"/>
-      <c r="N2692" s="47"/>
-      <c r="V2692" s="47"/>
-    </row>
-    <row r="2693" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2693" s="50"/>
-      <c r="N2693" s="47"/>
-      <c r="V2693" s="47"/>
-    </row>
-    <row r="2694" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2694" s="50"/>
-      <c r="N2694" s="47"/>
-      <c r="V2694" s="47"/>
-    </row>
-    <row r="2695" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2695" s="50"/>
-      <c r="N2695" s="47"/>
-      <c r="V2695" s="47"/>
-    </row>
-    <row r="2696" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2696" s="50"/>
-      <c r="N2696" s="47"/>
-      <c r="V2696" s="47"/>
-    </row>
-    <row r="2697" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2697" s="50"/>
-      <c r="N2697" s="47"/>
-      <c r="V2697" s="47"/>
-    </row>
-    <row r="2698" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2698" s="50"/>
-      <c r="N2698" s="47"/>
-      <c r="V2698" s="47"/>
-    </row>
-    <row r="2699" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2699" s="50"/>
-      <c r="N2699" s="47"/>
-      <c r="V2699" s="47"/>
-    </row>
-    <row r="2700" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2700" s="50"/>
-      <c r="N2700" s="47"/>
-      <c r="V2700" s="47"/>
-    </row>
-    <row r="2701" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2701" s="50"/>
-      <c r="N2701" s="47"/>
-      <c r="V2701" s="47"/>
-    </row>
-    <row r="2702" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2702" s="50"/>
-      <c r="N2702" s="47"/>
-      <c r="V2702" s="47"/>
-    </row>
-    <row r="2703" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2703" s="50"/>
-      <c r="N2703" s="47"/>
-      <c r="V2703" s="47"/>
-    </row>
-    <row r="2704" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2704" s="50"/>
-      <c r="N2704" s="47"/>
-      <c r="V2704" s="47"/>
-    </row>
-    <row r="2705" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2705" s="50"/>
-      <c r="N2705" s="47"/>
-      <c r="V2705" s="47"/>
-    </row>
-    <row r="2706" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2706" s="50"/>
-      <c r="N2706" s="47"/>
-      <c r="V2706" s="47"/>
-    </row>
-    <row r="2707" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2707" s="50"/>
-      <c r="N2707" s="47"/>
-      <c r="V2707" s="47"/>
-    </row>
-    <row r="2708" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2708" s="50"/>
-      <c r="N2708" s="47"/>
-      <c r="V2708" s="47"/>
-    </row>
-    <row r="2709" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2709" s="50"/>
-      <c r="N2709" s="47"/>
-      <c r="V2709" s="47"/>
-    </row>
-    <row r="2710" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2710" s="50"/>
-      <c r="N2710" s="47"/>
-      <c r="V2710" s="47"/>
-    </row>
-    <row r="2711" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2711" s="50"/>
-      <c r="N2711" s="47"/>
-      <c r="V2711" s="47"/>
-    </row>
-    <row r="2712" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2712" s="50"/>
-      <c r="N2712" s="47"/>
-      <c r="V2712" s="47"/>
-    </row>
-    <row r="2713" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2713" s="50"/>
-      <c r="N2713" s="47"/>
-      <c r="V2713" s="47"/>
-    </row>
-    <row r="2714" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2714" s="50"/>
-      <c r="N2714" s="47"/>
-      <c r="V2714" s="47"/>
-    </row>
-    <row r="2715" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2715" s="50"/>
-      <c r="N2715" s="47"/>
-      <c r="V2715" s="47"/>
-    </row>
-    <row r="2716" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2716" s="50"/>
-      <c r="N2716" s="47"/>
-      <c r="V2716" s="47"/>
-    </row>
-    <row r="2717" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2717" s="50"/>
-      <c r="N2717" s="47"/>
-      <c r="V2717" s="47"/>
-    </row>
-    <row r="2718" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2718" s="50"/>
-      <c r="N2718" s="47"/>
-      <c r="V2718" s="47"/>
-    </row>
-    <row r="2719" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2719" s="50"/>
-      <c r="N2719" s="47"/>
-      <c r="V2719" s="47"/>
-    </row>
-    <row r="2720" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2720" s="50"/>
-      <c r="N2720" s="47"/>
-      <c r="V2720" s="47"/>
-    </row>
-    <row r="2721" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2721" s="50"/>
-      <c r="N2721" s="47"/>
-      <c r="V2721" s="47"/>
-    </row>
-    <row r="2722" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2722" s="50"/>
-      <c r="N2722" s="47"/>
-      <c r="V2722" s="47"/>
-    </row>
-    <row r="2723" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2723" s="50"/>
-      <c r="N2723" s="47"/>
-      <c r="V2723" s="47"/>
-    </row>
-    <row r="2724" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2724" s="50"/>
-      <c r="N2724" s="47"/>
-      <c r="V2724" s="47"/>
-    </row>
-    <row r="2725" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2725" s="50"/>
-      <c r="N2725" s="47"/>
-      <c r="V2725" s="47"/>
-    </row>
-    <row r="2726" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2726" s="50"/>
-      <c r="N2726" s="47"/>
-      <c r="V2726" s="47"/>
-    </row>
-    <row r="2727" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2727" s="50"/>
-      <c r="N2727" s="47"/>
-      <c r="V2727" s="47"/>
-    </row>
-    <row r="2728" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I2728" s="50"/>
-      <c r="N2728" s="47"/>
-      <c r="V2728" s="47"/>
+        <v>1164</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="C1:V2124" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
nmv 02 04 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57AE6C6-6139-4FD9-9242-B34BAC07126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68632173-E38A-4A85-BA4B-E08E513C090C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3976,7 +3976,7 @@
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4262,9 +4262,9 @@
   <dimension ref="A1:V2124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2111" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1794" sqref="N1794"/>
+      <selection pane="bottomLeft" activeCell="N1283" sqref="N1283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
nmv 10 04 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.3 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4341609-C744-4BCB-9259-24800743E616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674EBCB4-319F-40BC-B730-8F5BE2DE5049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5453" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5455" uniqueCount="1182">
   <si>
     <t>Passage</t>
   </si>
@@ -3796,7 +3796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3975,6 +3975,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4259,9 +4262,9 @@
   <dimension ref="A1:V2124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1964" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1977" sqref="N1977"/>
+      <selection pane="bottomLeft" activeCell="N396" sqref="N396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -18916,8 +18919,12 @@
       <c r="P396" s="8"/>
       <c r="Q396" s="8"/>
       <c r="R396" s="8"/>
-      <c r="S396" s="8"/>
-      <c r="T396" s="8"/>
+      <c r="S396" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="T396" s="61" t="s">
+        <v>75</v>
+      </c>
       <c r="U396" s="8"/>
       <c r="V396" s="47"/>
     </row>

</xml_diff>